<commit_message>
originacion libre inversion completo
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C3909E-EDD8-4AC7-BBCF-295990A92021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0321ACA-5CCD-450C-AA95-19B3F3FDC378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="15" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="15" windowWidth="20730" windowHeight="11160" tabRatio="821" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimuladorAsesor" sheetId="10" r:id="rId1"/>
@@ -19,6 +19,15 @@
     <sheet name="ClientesBienvenida" sheetId="13" r:id="rId4"/>
     <sheet name="CreditosVisacion" sheetId="14" r:id="rId5"/>
     <sheet name="Desembolso" sheetId="15" r:id="rId6"/>
+    <sheet name="SimuladorAsesorCCS" sheetId="16" r:id="rId7"/>
+    <sheet name="SolicitudCreditoCCS" sheetId="17" r:id="rId8"/>
+    <sheet name="AnalisisCreditoCCS" sheetId="19" r:id="rId9"/>
+    <sheet name="ClientesBienvenidaCCS" sheetId="20" r:id="rId10"/>
+    <sheet name="CreditosVisacionCCS" sheetId="21" r:id="rId11"/>
+    <sheet name="DesembolsoCarteraCCS" sheetId="22" r:id="rId12"/>
+    <sheet name="VisacionCarteraCCS" sheetId="23" r:id="rId13"/>
+    <sheet name="DesembolsoSaneamientoCCS" sheetId="24" r:id="rId14"/>
+    <sheet name="DesembolsoCCS" sheetId="25" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="149">
   <si>
     <t>Cedula</t>
   </si>
@@ -378,6 +387,114 @@
   </si>
   <si>
     <t>"Remanentes - 60237038927 - REMANENTE"</t>
+  </si>
+  <si>
+    <t>"ALCALDIA MUNICIPAL DE MANIZALES NÓMINA JUBILADOS"</t>
+  </si>
+  <si>
+    <t>"Bogotá Centro"</t>
+  </si>
+  <si>
+    <t>"12"</t>
+  </si>
+  <si>
+    <t>"17000000"</t>
+  </si>
+  <si>
+    <t>"25"</t>
+  </si>
+  <si>
+    <t>"4500000"</t>
+  </si>
+  <si>
+    <t>"50000"</t>
+  </si>
+  <si>
+    <t>"3000000"</t>
+  </si>
+  <si>
+    <t>"70500000"</t>
+  </si>
+  <si>
+    <t>"930000"</t>
+  </si>
+  <si>
+    <t>"10/01/2009"</t>
+  </si>
+  <si>
+    <t>"carlos123@mail.com"</t>
+  </si>
+  <si>
+    <t>"3125117717"</t>
+  </si>
+  <si>
+    <t>"Tolima"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciudad </t>
+  </si>
+  <si>
+    <t>"Espinal"</t>
+  </si>
+  <si>
+    <t>Cartera1</t>
+  </si>
+  <si>
+    <t>Saneamiento2</t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t>"830000"</t>
+  </si>
+  <si>
+    <t>"19/10/2021"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cedula       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monto       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartera1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rutaPDF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cedula      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monto       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saneamiento2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"9777757" </t>
+  </si>
+  <si>
+    <t>"25000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saneamiento2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rutaPDF  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">entidad </t>
+  </si>
+  <si>
+    <t>"8300538122 -  FIDEICOMISO SOLUCIONES"</t>
   </si>
 </sst>
 </file>
@@ -422,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -434,6 +551,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -916,12 +1034,289 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788ABF16-704D-4D24-A7D1-A3757F9BD445}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD11F5D3-07F8-422D-AB89-8FE2C0A92130}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5C9861-FD03-4908-8AC1-7903766539F2}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9F8BE2-3D12-4A2D-B7AF-F8E6F2CE9D52}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCA4F98-63A6-4F65-A926-4DE1655E30DE}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752568D9-F8F8-47CF-8D4F-3A5B841BD0CC}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22B4C4B-A130-4E00-A807-2324C2C83647}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1525,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1622,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1665,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0416744F-FD4B-4063-9C82-0B43A550B273}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,4 +1742,499 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC7558A-6DD3-4212-BAB4-0FE9FA09F3EE}">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" t="s">
+        <v>121</v>
+      </c>
+      <c r="O2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="T2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E2D13F-DBFD-48EB-81E6-BFE85F296F36}">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" t="s">
+        <v>82</v>
+      </c>
+      <c r="X2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C7BDCE-01FA-4396-AD76-BA3CCCAF6C9A}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
originacion referencias digicredito avance 1
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683178A8-0869-4BBC-84AF-742BF724C286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB91374-E27B-4B72-B3A8-BCDE8BD838CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
     <sheet name="OriginacionCCS" sheetId="16" r:id="rId2"/>
+    <sheet name="OriginacionDigiCredito" sheetId="17" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="124">
   <si>
     <t>Cedula</t>
   </si>
@@ -392,6 +393,21 @@
   </si>
   <si>
     <t>"upper('Desembolso egreso'), upper('Desembolso activación de crédito')"</t>
+  </si>
+  <si>
+    <t>NumRadicadoCredito</t>
+  </si>
+  <si>
+    <t>"ALEYDA"</t>
+  </si>
+  <si>
+    <t>"Jubilados"</t>
+  </si>
+  <si>
+    <t>"86262"</t>
+  </si>
+  <si>
+    <t>"86260"</t>
   </si>
 </sst>
 </file>
@@ -469,7 +485,17 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -777,10 +803,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AW2"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AV1" sqref="AV1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AP1" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +819,7 @@
     <col min="46" max="16384" width="12.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -941,8 +967,11 @@
       <c r="AW1" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="AX1" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -980,7 +1009,7 @@
         <v>68</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>41</v>
@@ -1016,7 +1045,7 @@
         <v>38</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>40</v>
@@ -1089,11 +1118,14 @@
       </c>
       <c r="AW2" s="2" t="s">
         <v>117</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="AA2" r:id="rId1" display="prueba123@gmail.com" xr:uid="{68C5CA67-349F-451E-87B3-1675F58DE642}"/>
@@ -1434,11 +1466,336 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:XFD1048576 A1:AU2 AZ1:XFD2">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AY2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
+  <dimension ref="A1:AX2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AX2" sqref="AX2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="AA2" r:id="rId1" display="prueba123@gmail.com" xr:uid="{6713827F-A9FB-4336-B01B-35AD208A54F6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalizacion del flujo basico de digicredito coreccion error email
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB91374-E27B-4B72-B3A8-BCDE8BD838CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0659BA42-5522-4CFE-947C-4648B30C4DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="15" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -407,7 +407,7 @@
     <t>"86262"</t>
   </si>
   <si>
-    <t>"86260"</t>
+    <t>"86273"</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Flujo originación con compra cartera hasta analisis
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0659BA42-5522-4CFE-947C-4648B30C4DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F27C7-A774-4CF1-B4D5-2B38EC612E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="15" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="132">
   <si>
     <t>Cedula</t>
   </si>
@@ -407,7 +407,31 @@
     <t>"86262"</t>
   </si>
   <si>
-    <t>"86273"</t>
+    <t>"86313"</t>
+  </si>
+  <si>
+    <t>"52912399"</t>
+  </si>
+  <si>
+    <t>"RODRIGUEZ"</t>
+  </si>
+  <si>
+    <t>"GONZALEZ"</t>
+  </si>
+  <si>
+    <t>"25/Nov/2021"</t>
+  </si>
+  <si>
+    <t>"50"</t>
+  </si>
+  <si>
+    <t>"250000"</t>
+  </si>
+  <si>
+    <t>"8500000"</t>
+  </si>
+  <si>
+    <t>"300000"</t>
   </si>
 </sst>
 </file>
@@ -1479,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>52</v>
@@ -1651,22 +1675,22 @@
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="K2" t="s">
         <v>66</v>
@@ -1678,19 +1702,19 @@
         <v>120</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>108</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="R2" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Pruebas y ajustes flujo Digicredito - ABACUS
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8243B6-3F62-446B-8BDB-57E81BFD5C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477B9139-E4CA-44CA-AFD7-33752CBFEBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="130">
   <si>
     <t>Cedula</t>
   </si>
@@ -131,24 +131,9 @@
     <t>"1.8"</t>
   </si>
   <si>
-    <t>"36"</t>
-  </si>
-  <si>
     <t>"20000000"</t>
   </si>
   <si>
-    <t>"21"</t>
-  </si>
-  <si>
-    <t>"6500000"</t>
-  </si>
-  <si>
-    <t>"480000"</t>
-  </si>
-  <si>
-    <t>"90000"</t>
-  </si>
-  <si>
     <t>"20500000"</t>
   </si>
   <si>
@@ -404,12 +389,6 @@
     <t>"Jubilados"</t>
   </si>
   <si>
-    <t>"86262"</t>
-  </si>
-  <si>
-    <t>"86313"</t>
-  </si>
-  <si>
     <t>"52912399"</t>
   </si>
   <si>
@@ -438,6 +417,15 @@
   </si>
   <si>
     <t>"200000"</t>
+  </si>
+  <si>
+    <t>"86372"</t>
+  </si>
+  <si>
+    <t>"8700000"</t>
+  </si>
+  <si>
+    <t>"ALCALDÍA DE FLORENCIA ACTIVOS"</t>
   </si>
 </sst>
 </file>
@@ -836,7 +824,7 @@
   <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AP1" sqref="A1:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,19 +869,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -902,7 +890,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -947,114 +935,114 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL1" t="s">
         <v>93</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AM1" t="s">
         <v>94</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AN1" t="s">
         <v>95</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AO1" t="s">
         <v>96</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" t="s">
         <v>97</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>98</v>
       </c>
-      <c r="AM1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AR1" t="s">
         <v>100</v>
       </c>
-      <c r="AO1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>105</v>
-      </c>
       <c r="AS1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AV1" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AW1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" t="s">
         <v>66</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" t="s">
-        <v>71</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -1063,94 +1051,94 @@
         <v>29</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AL2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM2" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AN2" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AO2" t="s">
         <v>57</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AP2" t="s">
         <v>58</v>
       </c>
-      <c r="AL2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>62</v>
       </c>
-      <c r="AP2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>67</v>
-      </c>
       <c r="AR2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="AS2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="AT2" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="AU2" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1240,13 +1228,13 @@
         <v>19</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>21</v>
@@ -1270,87 +1258,87 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH1" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AI1" t="s">
         <v>94</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AJ1" t="s">
         <v>95</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AK1" t="s">
         <v>96</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AL1" t="s">
         <v>97</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AM1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" t="s">
         <v>100</v>
       </c>
-      <c r="AK1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AS1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AN1" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP1" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AT1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU1" t="s">
         <v>104</v>
       </c>
-      <c r="AR1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU1" t="s">
+      <c r="AV1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AY1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -1359,139 +1347,139 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>103</v>
+      </c>
+      <c r="V2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" t="s">
-        <v>108</v>
-      </c>
-      <c r="V2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="AW2" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AX2" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1509,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,19 +1535,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -1568,7 +1556,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -1613,120 +1601,120 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL1" t="s">
         <v>93</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AM1" t="s">
         <v>94</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AN1" t="s">
         <v>95</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AO1" t="s">
         <v>96</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" t="s">
         <v>97</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AQ1" t="s">
         <v>98</v>
       </c>
-      <c r="AM1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AR1" t="s">
         <v>100</v>
       </c>
-      <c r="AO1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>105</v>
-      </c>
       <c r="AS1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AV1" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="AW1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AX1" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="AY1" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" t="s">
         <v>120</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="R2" t="s">
-        <v>127</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -1735,100 +1723,100 @@
         <v>29</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AL2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM2" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AN2" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AO2" t="s">
         <v>57</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AP2" t="s">
         <v>58</v>
       </c>
-      <c r="AL2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>62</v>
       </c>
-      <c r="AP2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>67</v>
-      </c>
       <c r="AR2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="AS2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="AT2" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="AU2" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste Simulador interno: Valor seguros iniciales
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9604E5B8-9621-40E7-8ED9-52D54D84F185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3B891D-0344-4CBD-B563-F97FA7AAD723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="128">
   <si>
     <t>Cedula</t>
   </si>
@@ -245,9 +245,6 @@
     <t>"Remanentes - 60237038927 - REMANENTE"</t>
   </si>
   <si>
-    <t>"ALCALDIA MUNICIPAL DE MANIZALES NÓMINA JUBILADOS"</t>
-  </si>
-  <si>
     <t>"Bogotá Centro"</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
     <t>"70500000"</t>
   </si>
   <si>
-    <t>"930000"</t>
-  </si>
-  <si>
     <t>"10/01/2009"</t>
   </si>
   <si>
@@ -287,9 +281,6 @@
     <t>Saneamiento2</t>
   </si>
   <si>
-    <t>"100000"</t>
-  </si>
-  <si>
     <t>"830000"</t>
   </si>
   <si>
@@ -426,6 +417,9 @@
   </si>
   <si>
     <t>"ALCALDÍA DE FLORENCIA ACTIVOS"</t>
+  </si>
+  <si>
+    <t>"1030000"</t>
   </si>
 </sst>
 </file>
@@ -823,8 +817,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +866,7 @@
         <v>60</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>59</v>
@@ -881,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -935,58 +929,58 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>97</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>100</v>
       </c>
       <c r="AS1" t="s">
         <v>67</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AU1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1003,22 +997,22 @@
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="K2" t="s">
         <v>61</v>
@@ -1033,7 +1027,7 @@
         <v>36</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>37</v>
@@ -1063,7 +1057,7 @@
         <v>33</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>35</v>
@@ -1120,25 +1114,25 @@
         <v>62</v>
       </c>
       <c r="AR2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AS2" t="s">
         <v>68</v>
       </c>
       <c r="AT2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AU2" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="AV2" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1157,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC7558A-6DD3-4212-BAB4-0FE9FA09F3EE}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,7 +1228,7 @@
         <v>20</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>21</v>
@@ -1258,52 +1252,52 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF1" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>94</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>97</v>
       </c>
       <c r="AM1" s="7" t="s">
         <v>60</v>
       </c>
       <c r="AN1" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AO1" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AP1" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AQ1" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AR1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AS1" s="7" t="s">
         <v>65</v>
@@ -1312,24 +1306,24 @@
         <v>67</v>
       </c>
       <c r="AU1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1338,7 +1332,7 @@
         <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -1347,28 +1341,28 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
       </c>
       <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
         <v>71</v>
-      </c>
-      <c r="J2" t="s">
-        <v>72</v>
       </c>
       <c r="K2" t="s">
         <v>33</v>
       </c>
       <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" t="s">
         <v>73</v>
       </c>
-      <c r="M2" t="s">
-        <v>74</v>
-      </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="O2" t="s">
         <v>45</v>
@@ -1380,7 +1374,7 @@
         <v>34</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="S2" t="s">
         <v>36</v>
@@ -1389,7 +1383,7 @@
         <v>36</v>
       </c>
       <c r="U2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="V2" t="s">
         <v>37</v>
@@ -1398,16 +1392,16 @@
         <v>38</v>
       </c>
       <c r="X2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z2" t="s">
         <v>77</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>78</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>80</v>
       </c>
       <c r="AB2" t="s">
         <v>43</v>
@@ -1446,40 +1440,40 @@
         <v>61</v>
       </c>
       <c r="AN2" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="AO2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AP2" t="s">
         <v>62</v>
       </c>
       <c r="AQ2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AR2" t="s">
         <v>64</v>
       </c>
       <c r="AS2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="AT2" t="s">
         <v>68</v>
       </c>
       <c r="AU2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AV2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AW2" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="AX2" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +1491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <selection activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
@@ -1538,7 +1532,7 @@
         <v>60</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>59</v>
@@ -1547,7 +1541,7 @@
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -1601,72 +1595,72 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>97</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>100</v>
       </c>
       <c r="AS1" t="s">
         <v>67</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AU1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>47</v>
@@ -1675,22 +1669,22 @@
         <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="K2" t="s">
         <v>61</v>
@@ -1699,22 +1693,22 @@
         <v>63</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="R2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -1735,7 +1729,7 @@
         <v>33</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>35</v>
@@ -1792,31 +1786,31 @@
         <v>62</v>
       </c>
       <c r="AR2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AS2" t="s">
         <v>68</v>
       </c>
       <c r="AT2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AU2" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="AV2" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se corrige el error por el cual no se seleccionaba el monto correcto en la lista deplegable correspondiente al sanemaiento con la entidad PAN AMERICAN, para lo cual se agrega la logica de conversion del monto al tipo de dato disponible en el listado. Los cambios aplican para originacionCCS y Retanqueo CCS
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\ana.desarrollo59\Documents\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E6E7B8-CBF5-48B6-AB7D-5D27DD2D4098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E582805-FD32-4BDF-ACE0-1D200E97BE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20490" yWindow="1560" windowWidth="28830" windowHeight="7830" activeTab="2" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -3900,7 +3900,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="139">
   <si>
     <t>Cedula</t>
   </si>
@@ -4157,15 +4157,9 @@
     <t>"830000"</t>
   </si>
   <si>
-    <t>"19/10/2021"</t>
-  </si>
-  <si>
     <t>"8300538122 -  FIDEICOMISO SOLUCIONES"</t>
   </si>
   <si>
-    <t>"19/Oct/2021"</t>
-  </si>
-  <si>
     <t>DestinoCredito</t>
   </si>
   <si>
@@ -4308,6 +4302,21 @@
   </si>
   <si>
     <t>"Educación propia"</t>
+  </si>
+  <si>
+    <t>"2022"</t>
+  </si>
+  <si>
+    <t>"10/05/2022"</t>
+  </si>
+  <si>
+    <t>"05/Ene/2022"</t>
+  </si>
+  <si>
+    <t>05/01/2022</t>
+  </si>
+  <si>
+    <t>"Enero"</t>
   </si>
 </sst>
 </file>
@@ -4922,7 +4931,7 @@
         <v>64</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>63</v>
@@ -4931,7 +4940,7 @@
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -4985,58 +4994,58 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>96</v>
       </c>
-      <c r="AP1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>98</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>100</v>
       </c>
       <c r="AS1" t="s">
         <v>71</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AV1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5050,7 +5059,7 @@
         <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>30</v>
@@ -5083,7 +5092,7 @@
         <v>40</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>41</v>
@@ -5119,10 +5128,10 @@
         <v>39</v>
       </c>
       <c r="AA2" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>45</v>
@@ -5137,7 +5146,7 @@
         <v>48</v>
       </c>
       <c r="AG2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AH2" t="s">
         <v>54</v>
@@ -5170,25 +5179,25 @@
         <v>66</v>
       </c>
       <c r="AR2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AS2" s="11" t="s">
         <v>72</v>
       </c>
       <c r="AT2" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AU2" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AW2" s="2">
         <v>90537</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -5208,8 +5217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC7558A-6DD3-4212-BAB4-0FE9FA09F3EE}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5328,7 +5337,7 @@
         <v>20</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>21</v>
@@ -5352,34 +5361,34 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE1" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>95</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>97</v>
       </c>
       <c r="AM1" s="7" t="s">
         <v>64</v>
@@ -5391,13 +5400,13 @@
         <v>83</v>
       </c>
       <c r="AP1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR1" t="s">
         <v>98</v>
-      </c>
-      <c r="AQ1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>100</v>
       </c>
       <c r="AS1" s="7" t="s">
         <v>69</v>
@@ -5406,19 +5415,19 @@
         <v>71</v>
       </c>
       <c r="AU1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
@@ -5438,10 +5447,10 @@
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -5462,7 +5471,7 @@
         <v>78</v>
       </c>
       <c r="N2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>49</v>
@@ -5483,7 +5492,7 @@
         <v>40</v>
       </c>
       <c r="U2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="V2" t="s">
         <v>41</v>
@@ -5492,10 +5501,10 @@
         <v>42</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Y2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Z2" t="s">
         <v>80</v>
@@ -5537,43 +5546,43 @@
         <v>62</v>
       </c>
       <c r="AM2" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="AN2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AO2" t="s">
         <v>84</v>
       </c>
       <c r="AP2" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="AQ2" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="AR2" t="s">
         <v>68</v>
       </c>
       <c r="AS2" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="AT2" s="11" t="s">
         <v>72</v>
       </c>
       <c r="AU2" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AV2" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW2" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AX2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY2" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="AW2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -5596,7 +5605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+    <sheetView topLeftCell="AP1" workbookViewId="0">
       <selection activeCell="AW2" sqref="AW2"/>
     </sheetView>
   </sheetViews>
@@ -5690,7 +5699,7 @@
         <v>64</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>63</v>
@@ -5699,7 +5708,7 @@
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -5753,58 +5762,58 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>96</v>
       </c>
-      <c r="AP1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>98</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>100</v>
       </c>
       <c r="AS1" t="s">
         <v>71</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AV1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AY1" s="2" t="s">
         <v>82</v>
@@ -5818,31 +5827,31 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="K2" t="s">
         <v>65</v>
@@ -5851,22 +5860,22 @@
         <v>67</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R2" t="s">
         <v>119</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="R2" t="s">
-        <v>121</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -5887,7 +5896,7 @@
         <v>37</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>39</v>
@@ -5944,31 +5953,31 @@
         <v>66</v>
       </c>
       <c r="AR2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AS2" s="11" t="s">
         <v>72</v>
       </c>
       <c r="AT2" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="AU2" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AV2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AW2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AU2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="AX2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AY2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AZ2" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajuste error null referenciación en Originación y retanqueo
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\ana.desarrollo59\Documents\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E6E7B8-CBF5-48B6-AB7D-5D27DD2D4098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8D750C-D70C-4FA3-9EDF-74372C54BFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20490" yWindow="1560" windowWidth="28830" windowHeight="7830" activeTab="2" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -118,27 +118,27 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{C81C1A58-A5EF-46A5-AB5D-68A5FA72B860}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Tasa del Crédito;
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{AA373818-68A0-4F97-A8C2-C22BB82A5FD7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tasa del Credito;
 *Debe siempre estar a dos decimales.
 Eje:
 1.8 -&gt; 1.80</t>
@@ -374,28 +374,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{59E4785C-C6BA-4DB7-B854-7925BF3EAFD5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Primer nombre del Cliente;
-*Completo en mayúscula</t>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{5E4ED2BE-C801-4330-A627-D5E11EB4FD12}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nombre del Crédito;
+*Se recomienda usar el primer nombre del Cliente</t>
         </r>
       </text>
     </comment>
@@ -3900,7 +3900,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="145">
   <si>
     <t>Cedula</t>
   </si>
@@ -3992,24 +3992,9 @@
     <t>"Pensionado"</t>
   </si>
   <si>
-    <t>"36"</t>
-  </si>
-  <si>
     <t>"20000000"</t>
   </si>
   <si>
-    <t>"21"</t>
-  </si>
-  <si>
-    <t>"6500000"</t>
-  </si>
-  <si>
-    <t>"480000"</t>
-  </si>
-  <si>
-    <t>"90000"</t>
-  </si>
-  <si>
     <t>"20500000"</t>
   </si>
   <si>
@@ -4112,9 +4097,6 @@
     <t>fechaActual</t>
   </si>
   <si>
-    <t>"30/Sep/2021"</t>
-  </si>
-  <si>
     <t>Banco</t>
   </si>
   <si>
@@ -4304,10 +4286,55 @@
     <t>"1.80"</t>
   </si>
   <si>
-    <t>20/12/2021</t>
-  </si>
-  <si>
     <t>"Educación propia"</t>
+  </si>
+  <si>
+    <t>"05/01/2022"</t>
+  </si>
+  <si>
+    <t>"120"</t>
+  </si>
+  <si>
+    <t>"2022"</t>
+  </si>
+  <si>
+    <t>"10/Ene/1956"</t>
+  </si>
+  <si>
+    <t>"05/Ene/2022"</t>
+  </si>
+  <si>
+    <t>"6000000"</t>
+  </si>
+  <si>
+    <t>"8000000"</t>
+  </si>
+  <si>
+    <t>"600000"</t>
+  </si>
+  <si>
+    <t>"Enero"</t>
+  </si>
+  <si>
+    <t>"05/01/2000"</t>
+  </si>
+  <si>
+    <t>05/01/2022</t>
+  </si>
+  <si>
+    <t>"45460440"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"NAYIBE"</t>
+  </si>
+  <si>
+    <t>"CORRALES"</t>
+  </si>
+  <si>
+    <t>"MONTENEGRO"</t>
   </si>
 </sst>
 </file>
@@ -4438,7 +4465,17 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4828,8 +4865,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,19 +4956,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -4940,7 +4977,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -4985,114 +5022,114 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AN1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AO1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AP1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AR1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AS1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="AU1" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AV1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="R2" t="s">
         <v>133</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" t="s">
-        <v>70</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -5101,98 +5138,101 @@
         <v>29</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AL2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>131</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AR2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="AT2" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="AU2" s="12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="AW2" s="2">
         <v>90537</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:C2 E2:XFD2">
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
     <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -5209,7 +5249,7 @@
   <dimension ref="A1:AY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5322,13 +5362,13 @@
         <v>19</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>21</v>
@@ -5352,228 +5392,228 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI1" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AM1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AR1" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AS1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AN1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AT1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU1" t="s">
         <v>98</v>
       </c>
-      <c r="AQ1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AR1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AS1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="AW1" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AX1" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" t="s">
+        <v>97</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AU2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW2" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" t="s">
-        <v>128</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="S2" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" t="s">
-        <v>103</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU2" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="AY2" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5596,7 +5636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AW2" sqref="AW2"/>
     </sheetView>
   </sheetViews>
@@ -5687,19 +5727,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>21</v>
@@ -5708,7 +5748,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -5753,120 +5793,120 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM1" t="s">
         <v>88</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AN1" t="s">
         <v>89</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AO1" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AP1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AR1" t="s">
         <v>94</v>
       </c>
-      <c r="AN1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AS1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="AU1" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="AV1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AW1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="AY1" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" t="s">
         <v>115</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="R2" t="s">
-        <v>121</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -5875,100 +5915,100 @@
         <v>29</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AL2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" t="s">
         <v>53</v>
       </c>
-      <c r="AH2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AN2" t="s">
         <v>55</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AO2" t="s">
         <v>56</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AP2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AL2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AR2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="AT2" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="AU2" s="12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AV2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AX2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AW2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AZ2" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ2" s="14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambio camcluo remanente para desemboloso retanqueo
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8D750C-D70C-4FA3-9EDF-74372C54BFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAC2609-3667-4FCD-814B-460A52FE45BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -2574,7 +2574,7 @@
     <author>Analista Desarrollo59</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{0432A4FC-CAF5-4BB1-9FEB-210247790870}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{14EC37F8-B1CE-482C-91B1-03735921E8DC}">
       <text>
         <r>
           <rPr>
@@ -2598,7 +2598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{2286769F-0D07-45D8-80DB-BE9DEEF938AB}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{F9E8595A-23BA-4DB3-B46E-01018F1FA409}">
       <text>
         <r>
           <rPr>
@@ -2623,35 +2623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{3E6E4552-B3BF-45BD-96E9-46FCBB0B0435}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Año de nacimiento del cliente;
-*Debe estar en formato:
-DD/MM/AA
-*El mes con las primeras tres iniciales
-*El día menor a 10 debe iniciar con Cero.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{CF5D4E3E-E736-47E9-AB47-217C5409ADE7}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{55A53080-C1FB-40D6-A441-13CD31AFDCE5}">
       <text>
         <r>
           <rPr>
@@ -2678,7 +2650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{6BF746E7-3B7C-4313-828B-C465E542F452}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{69FE05B5-F12F-4829-8DDB-42C97E3E1EA8}">
       <text>
         <r>
           <rPr>
@@ -2703,7 +2675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{2A0432CF-2B76-4E0E-BFF9-374395E02AFF}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{C69CA3F5-DBD0-4CC6-A0AD-CBFE67BB8EEB}">
       <text>
         <r>
           <rPr>
@@ -2728,7 +2700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{302639EA-390E-433B-8A9D-5D11039B3B3D}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{3F4CCB1D-50CE-480D-9EC0-A6817C6F24F9}">
       <text>
         <r>
           <rPr>
@@ -2752,7 +2724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{917BEEC7-EE1D-4EBF-BE6A-E0780F094DF2}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{E454EBB3-EC80-485E-8ED0-E14D9DB199E6}">
       <text>
         <r>
           <rPr>
@@ -2777,7 +2749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{CE9F7C76-03EC-488B-8E6F-109A23608877}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{0B32431B-38A0-411A-A33E-EE806A4DEA7D}">
       <text>
         <r>
           <rPr>
@@ -2802,7 +2774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{BEBA9A11-2CDA-46C8-9508-97CC8B730156}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{FA1D7BE3-3B7F-4DCA-A4CE-BFD83D83DB02}">
       <text>
         <r>
           <rPr>
@@ -2827,7 +2799,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{2E7F3535-8F3C-45BF-91AE-915E311F3A85}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{32A1FAA3-720F-496E-9580-85EAF9357829}">
       <text>
         <r>
           <rPr>
@@ -2853,7 +2825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{7D624C2E-0431-417C-BCFF-5DB7F19FF3A2}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{6D03E615-84E8-4E68-8D53-2A506A82F15B}">
       <text>
         <r>
           <rPr>
@@ -2882,7 +2854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{3213DDD0-95A0-4547-A2F5-9CAFDCFB5DA9}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{7BBB61E6-D414-4208-B894-8498E90E6BF4}">
       <text>
         <r>
           <rPr>
@@ -2907,32 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{93E53B11-C10F-42C4-BE00-DC23E0931813}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Primer nombre del Cliente;
-*Completo en mayúscula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{A414C7B4-084A-4171-8FED-58C2F90FA64D}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{2A7DB574-2680-4F42-AA17-0273ED1652C5}">
       <text>
         <r>
           <rPr>
@@ -2957,7 +2904,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{805FE79B-8F40-47CF-BB25-426FFD4F41CB}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{35E3954E-27F5-4D8E-B5AE-2D92996B7CE3}">
       <text>
         <r>
           <rPr>
@@ -2982,7 +2929,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{D7809282-BFA9-4AF9-9BA9-1FEE6ABD428B}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{20BC2F34-9EB3-4DDE-AB8C-D9C818E510C5}">
       <text>
         <r>
           <rPr>
@@ -3007,7 +2954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{1F8BBE46-5916-4401-B6BD-AF25C2B2E7D3}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{28E6406B-75DE-4929-884A-6A1D0DE34633}">
       <text>
         <r>
           <rPr>
@@ -3035,7 +2982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{85D0D6D6-A42D-48A2-B0A9-38601EA7C95D}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{C446B284-3F79-416C-AF3A-9B8871C2AFDE}">
       <text>
         <r>
           <rPr>
@@ -3060,7 +3007,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{45C91CA4-E109-4C2B-99EA-F31E8F7386A8}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{A7757CBD-9E84-430F-8DC3-CDFEDDFCE724}">
       <text>
         <r>
           <rPr>
@@ -3086,7 +3033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{47A4873E-BBE0-42F2-9151-2FA7F0604B41}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{A0A984DB-EFCD-4EB0-AD27-77A82B4F56B4}">
       <text>
         <r>
           <rPr>
@@ -3111,7 +3058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{7AF9A4C4-655A-4CA0-870F-8CEF0DFE7E77}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{EBDFA775-CADD-43A0-9CCD-D5C9028C271D}">
       <text>
         <r>
           <rPr>
@@ -3136,57 +3083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{F4B15FB6-E05F-445B-B8CB-38FAC06DA700}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Revisar este campo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{62D45EB0-01FA-46D5-9077-4AAA2D741F92}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Colchón;
-Formato;
-*Sin puntos ni comas</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{9D3569F1-9F8D-4D17-988A-CC7951156090}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{8C9E7585-560E-4420-9EBE-3B97C6653B4F}">
       <text>
         <r>
           <rPr>
@@ -3211,7 +3108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{6D69B675-0A41-43B1-8D4E-72E859E34AB8}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{31837F90-3CD5-4B90-B6F2-CBA49035EA25}">
       <text>
         <r>
           <rPr>
@@ -3239,7 +3136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{90B42758-B336-4CEC-A342-8DDBC87954D7}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{D4D53531-DC1E-4991-A944-EF9D12182BA5}">
       <text>
         <r>
           <rPr>
@@ -3264,7 +3161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{BE89CA09-AF9A-45E9-ACED-64D7B4F8FF7B}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{3964D7D7-D3BF-4469-85CA-CA0F700EB0E2}">
       <text>
         <r>
           <rPr>
@@ -3289,7 +3186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{8798332F-0C5E-4144-837A-B7C5AB10A91D}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{D4CC3540-85F5-4050-A403-EEF8F25EA707}">
       <text>
         <r>
           <rPr>
@@ -3313,7 +3210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{14B2A9CD-3466-43E9-9D3B-E578329C299C}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{06A14CA3-47E2-47BB-BD32-9903BAF2CB6D}">
       <text>
         <r>
           <rPr>
@@ -3337,7 +3234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{0B290DC4-70CC-447A-8F02-C1D14BC58174}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{E97F49C8-820A-467F-9547-76B2E1939AA0}">
       <text>
         <r>
           <rPr>
@@ -3362,31 +3259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{2A3BA151-F14F-42DF-BA90-1B328658AB3C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Revisar este campo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{6EA5D7F6-F32C-4F78-80D4-44178FBF01BB}">
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{F0BC3096-6C97-4D4F-8AEC-42244F2A9649}">
       <text>
         <r>
           <rPr>
@@ -3410,7 +3283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{BDC4DEEB-AC36-4AD3-84FB-26538602023A}">
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{2EA7BF7F-A12D-45FB-9D2E-145C04B70564}">
       <text>
         <r>
           <rPr>
@@ -3437,7 +3310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{61F6DD0A-526B-4F34-996F-AECABC72CA7D}">
+    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{F0D0575B-FDEC-42F6-BED2-E89711FCF0A7}">
       <text>
         <r>
           <rPr>
@@ -3462,7 +3335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{93113E0D-9862-4BF7-A3A3-821852EBEAE6}">
+    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{01551780-738D-4966-AB01-08FB90C0B242}">
       <text>
         <r>
           <rPr>
@@ -3487,7 +3360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK2" authorId="0" shapeId="0" xr:uid="{CF80A25A-FDEF-4178-A5F1-01767740F1AA}">
+    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{50F40B8A-6A4B-4FEC-A5A3-F1079E220339}">
       <text>
         <r>
           <rPr>
@@ -3514,7 +3387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL2" authorId="0" shapeId="0" xr:uid="{FE77859D-1313-4C8A-9646-41EC27471FFB}">
+    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{5406339D-E896-4C6B-A6B2-0132B4229850}">
       <text>
         <r>
           <rPr>
@@ -3540,7 +3413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM2" authorId="0" shapeId="0" xr:uid="{E4744AA0-4AA7-4DAE-98D4-E658E8704603}">
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{DF12E362-0153-468B-8645-D3CEC67A88A0}">
       <text>
         <r>
           <rPr>
@@ -3566,7 +3439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN2" authorId="0" shapeId="0" xr:uid="{90E06E49-E249-45D3-A33E-96890C1F596B}">
+    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{58FB3D71-988A-4D3D-9B24-0BEE0868F88E}">
       <text>
         <r>
           <rPr>
@@ -3592,7 +3465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO2" authorId="0" shapeId="0" xr:uid="{3D837270-6AC1-4038-9049-FB7CDDCD9738}">
+    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{EDA8B302-4223-45EE-B80C-E61652C1E467}">
       <text>
         <r>
           <rPr>
@@ -3618,7 +3491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP2" authorId="0" shapeId="0" xr:uid="{726BBFE8-CC40-4907-9AD1-B0734F6C7827}">
+    <comment ref="AK2" authorId="0" shapeId="0" xr:uid="{80E78FEC-E9CF-4B3D-B074-0B3A0A348E11}">
       <text>
         <r>
           <rPr>
@@ -3642,7 +3515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ2" authorId="0" shapeId="0" xr:uid="{E4E9984B-80C9-404E-AEDD-F26EE05A5FE3}">
+    <comment ref="AL2" authorId="0" shapeId="0" xr:uid="{6ABE95F5-B956-43C6-AB3A-A5FECDCD5EDB}">
       <text>
         <r>
           <rPr>
@@ -3668,7 +3541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR2" authorId="0" shapeId="0" xr:uid="{DD692350-3FC1-45E6-8126-85573D20EB8F}">
+    <comment ref="AM2" authorId="0" shapeId="0" xr:uid="{3C4F35CB-15B9-4498-9D25-7F823334B549}">
       <text>
         <r>
           <rPr>
@@ -3693,7 +3566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS2" authorId="0" shapeId="0" xr:uid="{9119C30E-8BC2-41B1-B6A5-1B4759B6BB02}">
+    <comment ref="AN2" authorId="0" shapeId="0" xr:uid="{BC7AB2E0-EEA5-4836-A618-950FC472CB40}">
       <text>
         <r>
           <rPr>
@@ -3717,7 +3590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT2" authorId="0" shapeId="0" xr:uid="{2CAC2739-D516-4698-9DA6-056AB23D7BD3}">
+    <comment ref="AO2" authorId="0" shapeId="0" xr:uid="{8A525466-AD2C-4F9A-89D9-0570F5942A8B}">
       <text>
         <r>
           <rPr>
@@ -3741,7 +3614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU2" authorId="0" shapeId="0" xr:uid="{4A58FA51-76B2-4383-8E13-AC4CDC19CE6B}">
+    <comment ref="AP2" authorId="0" shapeId="0" xr:uid="{F3A92176-49D5-4586-968C-24AD737B34E3}">
       <text>
         <r>
           <rPr>
@@ -3765,7 +3638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV2" authorId="0" shapeId="0" xr:uid="{59745462-DAA9-4606-AD73-C85F30B634BC}">
+    <comment ref="AQ2" authorId="0" shapeId="0" xr:uid="{BDF5EE0A-1411-49FA-88D0-E9F89805BFA5}">
       <text>
         <r>
           <rPr>
@@ -3795,57 +3668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW2" authorId="0" shapeId="0" xr:uid="{91DB86FD-84BF-48A3-BD2E-60D70279DB30}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Numero de radicación de la solicitud.
-Consultarlo en base de datos.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AX2" authorId="0" shapeId="0" xr:uid="{34D60DD6-0369-4A66-A5B9-4618ED1AC685}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Numero de radicación del Crédito
-Consultarlo en base de datos.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AY2" authorId="0" shapeId="0" xr:uid="{70A86954-BA28-4C95-A46A-DE7E410B11D0}">
+    <comment ref="AR2" authorId="0" shapeId="0" xr:uid="{3C68A674-3190-4C9C-956C-8BF61409D6D1}">
       <text>
         <r>
           <rPr>
@@ -3870,7 +3693,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ2" authorId="0" shapeId="0" xr:uid="{A24CA455-2732-4951-BF89-082B66318026}">
+    <comment ref="AS2" authorId="0" shapeId="0" xr:uid="{0B412B49-E1E5-4894-9B26-17FDD4693346}">
       <text>
         <r>
           <rPr>
@@ -3900,7 +3723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="332">
   <si>
     <t>Cedula</t>
   </si>
@@ -4088,9 +3911,6 @@
     <t>"2021"</t>
   </si>
   <si>
-    <t>"05/10/2021"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "Efectivo" </t>
   </si>
   <si>
@@ -4247,9 +4067,6 @@
     <t>"GONZALEZ"</t>
   </si>
   <si>
-    <t>"25/Nov/2021"</t>
-  </si>
-  <si>
     <t>"50"</t>
   </si>
   <si>
@@ -4262,9 +4079,6 @@
     <t>"300000"</t>
   </si>
   <si>
-    <t>"7500000"</t>
-  </si>
-  <si>
     <t>"200000"</t>
   </si>
   <si>
@@ -4301,15 +4115,9 @@
     <t>"10/Ene/1956"</t>
   </si>
   <si>
-    <t>"05/Ene/2022"</t>
-  </si>
-  <si>
     <t>"6000000"</t>
   </si>
   <si>
-    <t>"8000000"</t>
-  </si>
-  <si>
     <t>"600000"</t>
   </si>
   <si>
@@ -4322,25 +4130,604 @@
     <t>05/01/2022</t>
   </si>
   <si>
-    <t>"45460440"</t>
-  </si>
-  <si>
-    <t>"P.A COLPENSIONES"</t>
-  </si>
-  <si>
-    <t>"NAYIBE"</t>
-  </si>
-  <si>
-    <t>"CORRALES"</t>
-  </si>
-  <si>
-    <t>"MONTENEGRO"</t>
+    <t>"SECRETARIA DISTRITAL DE INTEGRACIÓN SOCIAL"</t>
+  </si>
+  <si>
+    <t>"79290009"</t>
+  </si>
+  <si>
+    <t>"1.70"</t>
+  </si>
+  <si>
+    <t>"132"</t>
+  </si>
+  <si>
+    <t>"34500000"</t>
+  </si>
+  <si>
+    <t>"MIGUEL ANTONIO"</t>
+  </si>
+  <si>
+    <t>"MIGUEL"</t>
+  </si>
+  <si>
+    <t>"ANTONIO"</t>
+  </si>
+  <si>
+    <t>"TORRES"</t>
+  </si>
+  <si>
+    <t>"AMAYA"</t>
+  </si>
+  <si>
+    <t>"22/Feb/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pagaduria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cedula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plazo </t>
+  </si>
+  <si>
+    <t>montoSolicitado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DiasHabilesIntereses </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingresos  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> descLey  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> descNomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mes      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaDesembolso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> primerNombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> segundoNombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> primerApellido </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> segundoApellido </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaActual   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oficinaAsesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Actividad    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TotalActivos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vlrCompasSaneamientos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoContrato </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FechaIngreso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Celular      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> departamento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciudad      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rutaPDF                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DestinoCredito     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genero </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EstadoCivil </t>
+  </si>
+  <si>
+    <t>direccionResidencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoVivienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PapellidoReferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PnombreReferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TelefonoResidencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TelefonoTrabajo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Codigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnoAnalisis </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoDesen  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banco                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AccountingSource   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AccountingName                                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FechaRegistro </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartera1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saneamiento2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Credito </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombresApellidos           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contacto                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lineaCredito                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estadoActual </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> page </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> codigo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaExpedicion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estrado     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> claseVivienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> posicionHogar   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nivelEscolaridad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cuotaHipotecaria </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoDocNomina            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> otrosIngresos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> modalidadDesembolso      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoCliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> paisNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lugarDeNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nacionalidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> profesion   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mesesResidencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numeroHijos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> personasACargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoPension </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> codigoProgramaNomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaTerminacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nitAfiliacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoDocumento           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombreBeneficario    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> documentoBeneficiario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celularBeneficiario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> monedaExtranjera </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoTransanccion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> productoBancario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> banco       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numProducto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoProducto         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pais       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciudadExt </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> monto  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> moneda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> funcionarioPublico </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recursosPublicos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> expuestoPoliticamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaExpuesto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mes       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fecha        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnnoAfetacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaActual  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banco                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vinculo     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> plan     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tomarSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombresSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> parentescoSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pNombreRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sNombreRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pApellidoRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sApellidoRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relacionRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celRefP       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pNombreRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sNombreRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pApellidoRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sApellidoRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relacionRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celRefF      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> decisionExcepcion </t>
+  </si>
+  <si>
+    <t>"Soacha"</t>
+  </si>
+  <si>
+    <t>"Soltera/o"</t>
+  </si>
+  <si>
+    <t>"Arriendo"</t>
+  </si>
+  <si>
+    <t>"ALEYDA RODRIGUEZ GONZALEZ"</t>
+  </si>
+  <si>
+    <t>"15/02/1956"</t>
+  </si>
+  <si>
+    <t>"Entidad donde trabaja"</t>
+  </si>
+  <si>
+    <t>"Libre inversion"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"06/08/1976" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Estrato 1" </t>
+  </si>
+  <si>
+    <t>"Casa"</t>
+  </si>
+  <si>
+    <t>"Jefe de hogar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Universitario" </t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Desprendible de nómina" </t>
+  </si>
+  <si>
+    <t>"5000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Pago masivo (efectivo)" </t>
+  </si>
+  <si>
+    <t>"AAA"</t>
+  </si>
+  <si>
+    <t>"colombia"</t>
+  </si>
+  <si>
+    <t>"colombiano"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ingeniero" </t>
+  </si>
+  <si>
+    <t>"24"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"2"   </t>
+  </si>
+  <si>
+    <t>"pension"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"123456"  </t>
+  </si>
+  <si>
+    <t>"30/12/2022"</t>
+  </si>
+  <si>
+    <t>"123456"</t>
+  </si>
+  <si>
+    <t>"Certificación laboral"</t>
+  </si>
+  <si>
+    <t>"CEO"</t>
+  </si>
+  <si>
+    <t>"Luis Perez Ramirez"</t>
+  </si>
+  <si>
+    <t>"1234567890"</t>
+  </si>
+  <si>
+    <t>"3183903022"</t>
+  </si>
+  <si>
+    <t>"No"</t>
+  </si>
+  <si>
+    <t>"Importaciones"</t>
+  </si>
+  <si>
+    <t>"Santander"</t>
+  </si>
+  <si>
+    <t>"966855"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Inversiones en oro" </t>
+  </si>
+  <si>
+    <t>"Alemania"</t>
+  </si>
+  <si>
+    <t>"Berlin"</t>
+  </si>
+  <si>
+    <t>"8500"</t>
+  </si>
+  <si>
+    <t>"Euros"</t>
+  </si>
+  <si>
+    <t>"12/12/2008"</t>
+  </si>
+  <si>
+    <t>"Febrero"</t>
+  </si>
+  <si>
+    <t>"20/07/1963"</t>
+  </si>
+  <si>
+    <t>"16/02/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t>"Vinculado"</t>
+  </si>
+  <si>
+    <t>"Plan 1"</t>
+  </si>
+  <si>
+    <t>"Si"</t>
+  </si>
+  <si>
+    <t>"Juli Macias"</t>
+  </si>
+  <si>
+    <t>"Prima"</t>
+  </si>
+  <si>
+    <t>"maria"</t>
+  </si>
+  <si>
+    <t>"camila"</t>
+  </si>
+  <si>
+    <t>"lopez"</t>
+  </si>
+  <si>
+    <t>"cardenas"</t>
+  </si>
+  <si>
+    <t>"Amigo"</t>
+  </si>
+  <si>
+    <t>"3204567894"</t>
+  </si>
+  <si>
+    <t>"juan"</t>
+  </si>
+  <si>
+    <t>"david"</t>
+  </si>
+  <si>
+    <t>"reyes"</t>
+  </si>
+  <si>
+    <t>"sanchez"</t>
+  </si>
+  <si>
+    <t>"Hijo"</t>
+  </si>
+  <si>
+    <t>"3204047804"</t>
+  </si>
+  <si>
+    <t>NumRadicacion</t>
+  </si>
+  <si>
+    <t>"92840"</t>
+  </si>
+  <si>
+    <t>tipocontratoAbacus</t>
+  </si>
+  <si>
+    <t>"Pensionado por Invalidez"</t>
+  </si>
+  <si>
+    <t>"02/Marzo/2022"</t>
+  </si>
+  <si>
+    <t>29/10/2022</t>
+  </si>
+  <si>
+    <t>"05/05/2022"</t>
+  </si>
+  <si>
+    <t>"7349400"</t>
+  </si>
+  <si>
+    <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4424,15 +4811,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4458,6 +4842,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4465,7 +4853,107 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4865,8 +5353,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4884,7 +5372,7 @@
     <col min="11" max="11" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" style="2" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.140625" style="2" bestFit="1" customWidth="1"/>
@@ -4925,59 +5413,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="L1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="7" t="s">
-        <v>64</v>
+      <c r="R1" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -5022,105 +5510,105 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH1" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>84</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>85</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>86</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>87</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>88</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>89</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>90</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>92</v>
-      </c>
       <c r="AR1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AS1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AW1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AW1" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="K2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>143</v>
@@ -5129,7 +5617,7 @@
         <v>144</v>
       </c>
       <c r="R2" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>28</v>
@@ -5143,7 +5631,7 @@
       <c r="V2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="12" t="s">
         <v>44</v>
       </c>
       <c r="X2" s="2" t="s">
@@ -5153,13 +5641,13 @@
         <v>33</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>124</v>
+        <v>133</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>40</v>
@@ -5170,11 +5658,11 @@
       <c r="AE2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AF2" s="12" t="s">
         <v>43</v>
       </c>
       <c r="AG2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AH2" t="s">
         <v>49</v>
@@ -5200,40 +5688,40 @@
       <c r="AO2" t="s">
         <v>56</v>
       </c>
-      <c r="AP2" s="11" t="s">
+      <c r="AP2" s="10" t="s">
         <v>57</v>
       </c>
       <c r="AQ2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AR2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT2" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="AU2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>139</v>
+        <v>94</v>
+      </c>
+      <c r="AS2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT2" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU2" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV2" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="AW2" s="2">
         <v>90537</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:C2 E2:XFD2">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="AA2" r:id="rId1" display="prueba321@gmail.com" xr:uid="{68C5CA67-349F-451E-87B3-1675F58DE642}"/>
@@ -5307,13 +5795,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
@@ -5322,31 +5810,31 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="O1" t="s">
@@ -5361,19 +5849,19 @@
       <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="V1" s="7" t="s">
+      <c r="U1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
@@ -5392,78 +5880,78 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD1" t="s">
         <v>82</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>83</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>85</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>86</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>87</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>88</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>89</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>90</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="AM1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AR1" t="s">
         <v>93</v>
       </c>
-      <c r="AR1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AS1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT1" t="s">
         <v>64</v>
       </c>
-      <c r="AT1" t="s">
-        <v>65</v>
-      </c>
       <c r="AU1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AV1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AY1" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -5472,39 +5960,39 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
       </c>
       <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
         <v>69</v>
-      </c>
-      <c r="J2" t="s">
-        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>32</v>
       </c>
       <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
         <v>71</v>
       </c>
-      <c r="M2" t="s">
-        <v>72</v>
-      </c>
       <c r="N2" t="s">
-        <v>122</v>
-      </c>
-      <c r="O2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P2" t="s">
@@ -5513,8 +6001,8 @@
       <c r="Q2" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>73</v>
+      <c r="R2" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="S2" t="s">
         <v>35</v>
@@ -5523,7 +6011,7 @@
         <v>35</v>
       </c>
       <c r="U2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V2" t="s">
         <v>36</v>
@@ -5531,17 +6019,17 @@
       <c r="W2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="9" t="s">
-        <v>124</v>
+      <c r="X2" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="Y2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Z2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA2" t="s">
         <v>74</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>75</v>
       </c>
       <c r="AB2" t="s">
         <v>42</v>
@@ -5573,55 +6061,55 @@
       <c r="AK2" t="s">
         <v>56</v>
       </c>
-      <c r="AL2" s="11" t="s">
+      <c r="AL2" s="10" t="s">
         <v>57</v>
       </c>
       <c r="AM2" t="s">
         <v>60</v>
       </c>
       <c r="AN2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AO2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP2" t="s">
         <v>61</v>
       </c>
       <c r="AQ2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AR2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV2" s="12" t="s">
+      <c r="AV2" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW2" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AX2" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="AW2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX2" s="8" t="s">
+      <c r="AY2" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:XFD1048576 A1:AU2 AZ1:XFD2">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AY2">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="X2" r:id="rId1" display="dabogado@excelcredit.co" xr:uid="{0565F543-D6A3-457F-A02B-20E7DC298B68}"/>
@@ -5634,10 +6122,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:DN2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AW2" sqref="AW2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5646,8 +6134,8 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -5684,385 +6172,787 @@
     <col min="40" max="40" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="67.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+    <row r="1" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" t="s">
+        <v>159</v>
+      </c>
+      <c r="O1" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>162</v>
+      </c>
+      <c r="R1" t="s">
+        <v>163</v>
+      </c>
+      <c r="S1" t="s">
+        <v>164</v>
+      </c>
+      <c r="T1" t="s">
+        <v>165</v>
+      </c>
+      <c r="U1" t="s">
+        <v>166</v>
+      </c>
+      <c r="V1" t="s">
+        <v>167</v>
+      </c>
+      <c r="W1" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>26</v>
+      <c r="X1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>176</v>
       </c>
       <c r="AG1" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
       <c r="AH1" t="s">
-        <v>83</v>
+        <v>178</v>
       </c>
       <c r="AI1" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="AJ1" t="s">
-        <v>85</v>
+        <v>180</v>
       </c>
       <c r="AK1" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="AL1" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
       <c r="AM1" t="s">
-        <v>88</v>
+        <v>183</v>
       </c>
       <c r="AN1" t="s">
-        <v>89</v>
+        <v>184</v>
       </c>
       <c r="AO1" t="s">
-        <v>90</v>
+        <v>185</v>
       </c>
       <c r="AP1" t="s">
-        <v>91</v>
+        <v>186</v>
       </c>
       <c r="AQ1" t="s">
-        <v>92</v>
+        <v>187</v>
       </c>
       <c r="AR1" t="s">
-        <v>94</v>
+        <v>188</v>
       </c>
       <c r="AS1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>77</v>
+        <v>189</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>205</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>206</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>207</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>213</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>215</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>216</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>217</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>219</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>221</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>222</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>223</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>224</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>225</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>226</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>227</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>228</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>229</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>230</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>231</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>232</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>233</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>234</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>235</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>236</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>237</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>238</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>239</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>240</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>241</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>242</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>243</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>244</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>245</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>246</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>247</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>248</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>249</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>250</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>251</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>252</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>253</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>254</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>255</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>256</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>257</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>258</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>259</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>260</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>323</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" t="s">
+        <v>302</v>
+      </c>
+      <c r="K2" t="s">
+        <v>329</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="P2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="R2" t="s">
-        <v>115</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="AO2" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="AR2" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AS2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT2" t="s">
         <v>110</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT2" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="AU2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>111</v>
+      <c r="AU2" t="s">
+        <v>264</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>267</v>
       </c>
       <c r="AY2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AZ2" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AT3" s="8"/>
-      <c r="AU3" s="8"/>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>123</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>268</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>269</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>270</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>271</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>273</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>274</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>275</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>276</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>277</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>278</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>278</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>279</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>280</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>282</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>47</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>283</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>284</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>285</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>286</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>287</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>288</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>289</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>290</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>291</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>293</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>294</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>295</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>296</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>297</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>298</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>299</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>300</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>301</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>302</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>303</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>128</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>304</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>305</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>306</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>307</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>308</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>309</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>310</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>311</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>312</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>313</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>314</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>315</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>316</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>317</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>318</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>319</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>320</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>321</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>322</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>292</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>324</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>326</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A2:L2 BA2:XFD2">
-    <cfRule type="duplicateValues" dxfId="7" priority="12"/>
+  <conditionalFormatting sqref="CU2:XFD2 CB2 BY2 A1:XFD1">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:R2">
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:AR3">
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:AR2">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+  <conditionalFormatting sqref="C2:G2">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS3:AX3">
+  <conditionalFormatting sqref="H2:K2">
+    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:N2">
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:P2">
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:T2">
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:V2">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:AB2">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2:AE2">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF2:AG2">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH2:AL2">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM2">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN2">
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AX2">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  <conditionalFormatting sqref="AO2:AP2">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY3:AZ3">
+  <conditionalFormatting sqref="AQ2">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AY2:AZ2">
+  <conditionalFormatting sqref="AR2:AS2">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AA2" r:id="rId1" display="prueba321@gmail.com" xr:uid="{F92ACD0A-1AAC-4AF3-9653-782CACF011FF}"/>
+    <hyperlink ref="W2" r:id="rId1" display="prueba321@gmail.com" xr:uid="{0827CE73-83FA-4AC6-B5E7-8249E9A9C693}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se realiza el ajuste de la exepciones
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAC2609-3667-4FCD-814B-460A52FE45BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788BC6D0-6192-4D83-B06F-28C15F33A806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -3723,7 +3723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="337">
   <si>
     <t>Cedula</t>
   </si>
@@ -3809,916 +3809,931 @@
     <t>"9777757"</t>
   </si>
   <si>
+    <t>"Pensionado"</t>
+  </si>
+  <si>
+    <t>"20000000"</t>
+  </si>
+  <si>
+    <t>"20500000"</t>
+  </si>
+  <si>
+    <t>"360000"</t>
+  </si>
+  <si>
+    <t>"Pensionado por Tiempo (Vejez)"</t>
+  </si>
+  <si>
+    <t>"10/03/2000"</t>
+  </si>
+  <si>
+    <t>"CARLOS"</t>
+  </si>
+  <si>
+    <t>"HERRERA"</t>
+  </si>
+  <si>
+    <t>"ARBOLEDA"</t>
+  </si>
+  <si>
+    <t>"prueba123@gmail.com"</t>
+  </si>
+  <si>
+    <t>"3125127717"</t>
+  </si>
+  <si>
+    <t>"Cundinamarca"</t>
+  </si>
+  <si>
+    <t>"Anapoima"</t>
+  </si>
+  <si>
+    <t>"src/test/resources/Data/PDFPRUEBA.pdf"</t>
+  </si>
+  <si>
+    <t>"2021-04-20"</t>
+  </si>
+  <si>
+    <t>"xx"</t>
+  </si>
+  <si>
+    <t>"COLFONDOS"</t>
+  </si>
+  <si>
+    <t>"17/Mar/1956"</t>
+  </si>
+  <si>
+    <t>"0"</t>
+  </si>
+  <si>
+    <t>"Educacion propia"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>"Soltero"</t>
+  </si>
+  <si>
+    <t>"Calle 2d #22-52"</t>
+  </si>
+  <si>
+    <t>"FAMILIAR"</t>
+  </si>
+  <si>
+    <t>"alejandro"</t>
+  </si>
+  <si>
+    <t>"perez"</t>
+  </si>
+  <si>
+    <t>"7210273"</t>
+  </si>
+  <si>
+    <t>"9007146"</t>
+  </si>
+  <si>
+    <t>"3112"</t>
+  </si>
+  <si>
+    <t>NombreCredito</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>"Noviembre"</t>
+  </si>
+  <si>
+    <t>"2021"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Efectivo" </t>
+  </si>
+  <si>
+    <t>fechaActual</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>"Remanentes - 60237038927 - REMANENTE"</t>
+  </si>
+  <si>
+    <t>"ALCALDIA MUNICIPAL DE MANIZALES NÓMINA JUBILADOS"</t>
+  </si>
+  <si>
+    <t>"Bogotá Centro"</t>
+  </si>
+  <si>
+    <t>"25"</t>
+  </si>
+  <si>
+    <t>"4500000"</t>
+  </si>
+  <si>
+    <t>"50000"</t>
+  </si>
+  <si>
+    <t>"70500000"</t>
+  </si>
+  <si>
+    <t>"10/01/2009"</t>
+  </si>
+  <si>
+    <t>"Tolima"</t>
+  </si>
+  <si>
+    <t>"Espinal"</t>
+  </si>
+  <si>
+    <t>Cartera1</t>
+  </si>
+  <si>
+    <t>Saneamiento2</t>
+  </si>
+  <si>
+    <t>"830000"</t>
+  </si>
+  <si>
+    <t>"19/10/2021"</t>
+  </si>
+  <si>
+    <t>"8300538122 -  FIDEICOMISO SOLUCIONES"</t>
+  </si>
+  <si>
+    <t>"19/Oct/2021"</t>
+  </si>
+  <si>
+    <t>DestinoCredito</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>EstadoCivil</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>TipoVivienda</t>
+  </si>
+  <si>
+    <t>PapellidoReferencia</t>
+  </si>
+  <si>
+    <t>PnombreReferencia</t>
+  </si>
+  <si>
+    <t>TelefonoResidencia</t>
+  </si>
+  <si>
+    <t>TelefonoTrabajo</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>AnoAnalisis</t>
+  </si>
+  <si>
+    <t>fechaDesembolso</t>
+  </si>
+  <si>
+    <t>TipoDesen</t>
+  </si>
+  <si>
+    <t>"Efectivo"</t>
+  </si>
+  <si>
+    <t>Snombre</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>entidad</t>
+  </si>
+  <si>
+    <t>"90"</t>
+  </si>
+  <si>
+    <t>AccountingSource</t>
+  </si>
+  <si>
+    <t>AccountingName</t>
+  </si>
+  <si>
+    <t>FechaRegistro</t>
+  </si>
+  <si>
+    <t>NumRadicado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"'ACRED','EGRESO'" </t>
+  </si>
+  <si>
+    <t>29/10/2021</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>"upper('Desembolso egreso'), upper('Desembolso activación de crédito')"</t>
+  </si>
+  <si>
+    <t>NumRadicadoCredito</t>
+  </si>
+  <si>
+    <t>"ALEYDA"</t>
+  </si>
+  <si>
+    <t>"Jubilados"</t>
+  </si>
+  <si>
+    <t>"86313"</t>
+  </si>
+  <si>
+    <t>"52912399"</t>
+  </si>
+  <si>
+    <t>"RODRIGUEZ"</t>
+  </si>
+  <si>
+    <t>"GONZALEZ"</t>
+  </si>
+  <si>
+    <t>"50"</t>
+  </si>
+  <si>
+    <t>"250000"</t>
+  </si>
+  <si>
+    <t>"8500000"</t>
+  </si>
+  <si>
+    <t>"300000"</t>
+  </si>
+  <si>
+    <t>"200000"</t>
+  </si>
+  <si>
+    <t>"1030000"</t>
+  </si>
+  <si>
+    <t>"3125117718"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"prueba321@gmail.com" </t>
+  </si>
+  <si>
+    <t>"3125127718"</t>
+  </si>
+  <si>
+    <t>"12345"</t>
+  </si>
+  <si>
+    <t>"1.80"</t>
+  </si>
+  <si>
+    <t>"Educación propia"</t>
+  </si>
+  <si>
+    <t>"05/01/2022"</t>
+  </si>
+  <si>
+    <t>"2022"</t>
+  </si>
+  <si>
+    <t>"Enero"</t>
+  </si>
+  <si>
+    <t>"1.70"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pagaduria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cedula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plazo </t>
+  </si>
+  <si>
+    <t>montoSolicitado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DiasHabilesIntereses </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingresos  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> descLey  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> descNomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mes      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaDesembolso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> primerNombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> segundoNombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> primerApellido </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> segundoApellido </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaActual   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oficinaAsesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Actividad    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TotalActivos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vlrCompasSaneamientos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoContrato </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FechaIngreso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Celular      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> departamento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciudad      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rutaPDF                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DestinoCredito     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genero </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EstadoCivil </t>
+  </si>
+  <si>
+    <t>direccionResidencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoVivienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PapellidoReferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PnombreReferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TelefonoResidencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TelefonoTrabajo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Codigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnoAnalisis </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoDesen  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banco                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AccountingSource   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AccountingName                                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FechaRegistro </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartera1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saneamiento2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Credito </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombresApellidos           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contacto                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lineaCredito                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estadoActual </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> page </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> codigo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaExpedicion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estrado     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> claseVivienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> posicionHogar   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nivelEscolaridad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cuotaHipotecaria </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoDocNomina            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> otrosIngresos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> modalidadDesembolso      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoCliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> paisNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lugarDeNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nacionalidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> profesion   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mesesResidencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numeroHijos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> personasACargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoPension </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> codigoProgramaNomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaTerminacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nitAfiliacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoDocumento           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombreBeneficario    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> documentoBeneficiario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celularBeneficiario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> monedaExtranjera </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoTransanccion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> productoBancario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> banco       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numProducto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoProducto         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pais       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciudadExt </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> monto  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> moneda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> funcionarioPublico </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recursosPublicos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> expuestoPoliticamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaExpuesto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mes       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fecha        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnnoAfetacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaActual  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banco                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vinculo     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> plan     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tomarSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombresSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> parentescoSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pNombreRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sNombreRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pApellidoRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sApellidoRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relacionRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celRefP       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pNombreRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sNombreRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pApellidoRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sApellidoRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relacionRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celRefF      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> decisionExcepcion </t>
+  </si>
+  <si>
+    <t>"Soacha"</t>
+  </si>
+  <si>
+    <t>"Soltera/o"</t>
+  </si>
+  <si>
+    <t>"Arriendo"</t>
+  </si>
+  <si>
+    <t>"ALEYDA RODRIGUEZ GONZALEZ"</t>
+  </si>
+  <si>
+    <t>"15/02/1956"</t>
+  </si>
+  <si>
+    <t>"Entidad donde trabaja"</t>
+  </si>
+  <si>
+    <t>"Libre inversion"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"06/08/1976" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Estrato 1" </t>
+  </si>
+  <si>
+    <t>"Casa"</t>
+  </si>
+  <si>
+    <t>"Jefe de hogar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Universitario" </t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Desprendible de nómina" </t>
+  </si>
+  <si>
+    <t>"5000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Pago masivo (efectivo)" </t>
+  </si>
+  <si>
+    <t>"AAA"</t>
+  </si>
+  <si>
+    <t>"colombia"</t>
+  </si>
+  <si>
+    <t>"colombiano"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ingeniero" </t>
+  </si>
+  <si>
+    <t>"24"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"2"   </t>
+  </si>
+  <si>
+    <t>"pension"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"123456"  </t>
+  </si>
+  <si>
+    <t>"30/12/2022"</t>
+  </si>
+  <si>
+    <t>"123456"</t>
+  </si>
+  <si>
+    <t>"Certificación laboral"</t>
+  </si>
+  <si>
+    <t>"CEO"</t>
+  </si>
+  <si>
+    <t>"Luis Perez Ramirez"</t>
+  </si>
+  <si>
+    <t>"1234567890"</t>
+  </si>
+  <si>
+    <t>"3183903022"</t>
+  </si>
+  <si>
+    <t>"No"</t>
+  </si>
+  <si>
+    <t>"Importaciones"</t>
+  </si>
+  <si>
+    <t>"Santander"</t>
+  </si>
+  <si>
+    <t>"966855"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Inversiones en oro" </t>
+  </si>
+  <si>
+    <t>"Alemania"</t>
+  </si>
+  <si>
+    <t>"Berlin"</t>
+  </si>
+  <si>
+    <t>"8500"</t>
+  </si>
+  <si>
+    <t>"Euros"</t>
+  </si>
+  <si>
+    <t>"12/12/2008"</t>
+  </si>
+  <si>
+    <t>"Febrero"</t>
+  </si>
+  <si>
+    <t>"20/07/1963"</t>
+  </si>
+  <si>
+    <t>"16/02/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t>"Vinculado"</t>
+  </si>
+  <si>
+    <t>"Plan 1"</t>
+  </si>
+  <si>
+    <t>"Si"</t>
+  </si>
+  <si>
+    <t>"Juli Macias"</t>
+  </si>
+  <si>
+    <t>"Prima"</t>
+  </si>
+  <si>
+    <t>"maria"</t>
+  </si>
+  <si>
+    <t>"camila"</t>
+  </si>
+  <si>
+    <t>"lopez"</t>
+  </si>
+  <si>
+    <t>"cardenas"</t>
+  </si>
+  <si>
+    <t>"Amigo"</t>
+  </si>
+  <si>
+    <t>"3204567894"</t>
+  </si>
+  <si>
+    <t>"juan"</t>
+  </si>
+  <si>
+    <t>"david"</t>
+  </si>
+  <si>
+    <t>"reyes"</t>
+  </si>
+  <si>
+    <t>"sanchez"</t>
+  </si>
+  <si>
+    <t>"Hijo"</t>
+  </si>
+  <si>
+    <t>"3204047804"</t>
+  </si>
+  <si>
+    <t>NumRadicacion</t>
+  </si>
+  <si>
+    <t>"92840"</t>
+  </si>
+  <si>
+    <t>tipocontratoAbacus</t>
+  </si>
+  <si>
+    <t>"Pensionado por Invalidez"</t>
+  </si>
+  <si>
+    <t>"02/Marzo/2022"</t>
+  </si>
+  <si>
+    <t>29/10/2022</t>
+  </si>
+  <si>
+    <t>"05/05/2022"</t>
+  </si>
+  <si>
+    <t>"7349400"</t>
+  </si>
+  <si>
+    <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"51618664"</t>
+  </si>
+  <si>
+    <t>"10"</t>
+  </si>
+  <si>
+    <t>"6500000"</t>
+  </si>
+  <si>
+    <t>"350000"</t>
+  </si>
+  <si>
+    <t>"28/02/2022"</t>
+  </si>
+  <si>
+    <t>"OLGA"</t>
+  </si>
+  <si>
+    <t>"BEATRIZ"</t>
+  </si>
+  <si>
+    <t>"CONTRERAS"</t>
+  </si>
+  <si>
+    <t>"DE CAMACHO"</t>
+  </si>
+  <si>
+    <t>"2000001"</t>
+  </si>
+  <si>
+    <t>"prueba321@gmail.com"</t>
+  </si>
+  <si>
+    <t>"alejando"</t>
+  </si>
+  <si>
+    <t>"'ACRED','EGRESO'"</t>
+  </si>
+  <si>
+    <t>"upper('Desembolso egreso'),upper('Desembolso activación de crédito')"</t>
+  </si>
+  <si>
+    <t>"7/3/2022"</t>
+  </si>
+  <si>
+    <t>"20/Jun/1958"</t>
+  </si>
+  <si>
     <t>"Cartagena"</t>
   </si>
   <si>
-    <t>"Pensionado"</t>
-  </si>
-  <si>
-    <t>"20000000"</t>
-  </si>
-  <si>
-    <t>"20500000"</t>
-  </si>
-  <si>
-    <t>"360000"</t>
-  </si>
-  <si>
-    <t>"Pensionado por Tiempo (Vejez)"</t>
-  </si>
-  <si>
-    <t>"10/03/2000"</t>
-  </si>
-  <si>
-    <t>"CARLOS"</t>
-  </si>
-  <si>
-    <t>"HERRERA"</t>
-  </si>
-  <si>
-    <t>"ARBOLEDA"</t>
-  </si>
-  <si>
-    <t>"prueba123@gmail.com"</t>
-  </si>
-  <si>
-    <t>"3125127717"</t>
-  </si>
-  <si>
-    <t>"Cundinamarca"</t>
-  </si>
-  <si>
-    <t>"Anapoima"</t>
-  </si>
-  <si>
-    <t>"src/test/resources/Data/PDFPRUEBA.pdf"</t>
-  </si>
-  <si>
-    <t>"2021-04-20"</t>
-  </si>
-  <si>
-    <t>"xx"</t>
-  </si>
-  <si>
-    <t>"COLFONDOS"</t>
-  </si>
-  <si>
-    <t>"17/Mar/1956"</t>
-  </si>
-  <si>
-    <t>"0"</t>
-  </si>
-  <si>
-    <t>"Educacion propia"</t>
-  </si>
-  <si>
-    <t>"M"</t>
-  </si>
-  <si>
-    <t>"Soltero"</t>
-  </si>
-  <si>
-    <t>"Calle 2d #22-52"</t>
-  </si>
-  <si>
-    <t>"FAMILIAR"</t>
-  </si>
-  <si>
-    <t>"alejandro"</t>
-  </si>
-  <si>
-    <t>"perez"</t>
-  </si>
-  <si>
-    <t>"7210273"</t>
-  </si>
-  <si>
-    <t>"9007146"</t>
-  </si>
-  <si>
-    <t>"3112"</t>
-  </si>
-  <si>
-    <t>NombreCredito</t>
-  </si>
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>"Noviembre"</t>
-  </si>
-  <si>
-    <t>"2021"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Efectivo" </t>
-  </si>
-  <si>
-    <t>fechaActual</t>
-  </si>
-  <si>
-    <t>Banco</t>
-  </si>
-  <si>
-    <t>"Remanentes - 60237038927 - REMANENTE"</t>
-  </si>
-  <si>
-    <t>"ALCALDIA MUNICIPAL DE MANIZALES NÓMINA JUBILADOS"</t>
-  </si>
-  <si>
-    <t>"Bogotá Centro"</t>
-  </si>
-  <si>
-    <t>"25"</t>
-  </si>
-  <si>
-    <t>"4500000"</t>
-  </si>
-  <si>
-    <t>"50000"</t>
-  </si>
-  <si>
-    <t>"70500000"</t>
-  </si>
-  <si>
-    <t>"10/01/2009"</t>
-  </si>
-  <si>
-    <t>"Tolima"</t>
-  </si>
-  <si>
-    <t>"Espinal"</t>
-  </si>
-  <si>
-    <t>Cartera1</t>
-  </si>
-  <si>
-    <t>Saneamiento2</t>
-  </si>
-  <si>
-    <t>"830000"</t>
-  </si>
-  <si>
-    <t>"19/10/2021"</t>
-  </si>
-  <si>
-    <t>"8300538122 -  FIDEICOMISO SOLUCIONES"</t>
-  </si>
-  <si>
-    <t>"19/Oct/2021"</t>
-  </si>
-  <si>
-    <t>DestinoCredito</t>
-  </si>
-  <si>
-    <t>Sexo</t>
-  </si>
-  <si>
-    <t>EstadoCivil</t>
-  </si>
-  <si>
-    <t>Direccion</t>
-  </si>
-  <si>
-    <t>TipoVivienda</t>
-  </si>
-  <si>
-    <t>PapellidoReferencia</t>
-  </si>
-  <si>
-    <t>PnombreReferencia</t>
-  </si>
-  <si>
-    <t>TelefonoResidencia</t>
-  </si>
-  <si>
-    <t>TelefonoTrabajo</t>
-  </si>
-  <si>
-    <t>Codigo</t>
-  </si>
-  <si>
-    <t>AnoAnalisis</t>
-  </si>
-  <si>
-    <t>fechaDesembolso</t>
-  </si>
-  <si>
-    <t>TipoDesen</t>
-  </si>
-  <si>
-    <t>"Efectivo"</t>
-  </si>
-  <si>
-    <t>Snombre</t>
-  </si>
-  <si>
-    <t>""</t>
-  </si>
-  <si>
-    <t>entidad</t>
-  </si>
-  <si>
-    <t>"90"</t>
-  </si>
-  <si>
-    <t>AccountingSource</t>
-  </si>
-  <si>
-    <t>AccountingName</t>
-  </si>
-  <si>
-    <t>FechaRegistro</t>
-  </si>
-  <si>
-    <t>NumRadicado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"'ACRED','EGRESO'" </t>
-  </si>
-  <si>
-    <t>29/10/2021</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>"upper('Desembolso egreso'), upper('Desembolso activación de crédito')"</t>
-  </si>
-  <si>
-    <t>NumRadicadoCredito</t>
-  </si>
-  <si>
-    <t>"ALEYDA"</t>
-  </si>
-  <si>
-    <t>"Jubilados"</t>
-  </si>
-  <si>
-    <t>"86313"</t>
-  </si>
-  <si>
-    <t>"52912399"</t>
-  </si>
-  <si>
-    <t>"RODRIGUEZ"</t>
-  </si>
-  <si>
-    <t>"GONZALEZ"</t>
-  </si>
-  <si>
-    <t>"50"</t>
-  </si>
-  <si>
-    <t>"250000"</t>
-  </si>
-  <si>
-    <t>"8500000"</t>
-  </si>
-  <si>
-    <t>"300000"</t>
-  </si>
-  <si>
-    <t>"200000"</t>
-  </si>
-  <si>
-    <t>"1030000"</t>
-  </si>
-  <si>
-    <t>"3125117718"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"prueba321@gmail.com" </t>
-  </si>
-  <si>
-    <t>"3125127718"</t>
-  </si>
-  <si>
-    <t>"12345"</t>
-  </si>
-  <si>
-    <t>"1.80"</t>
-  </si>
-  <si>
-    <t>"Educación propia"</t>
-  </si>
-  <si>
-    <t>"05/01/2022"</t>
+    <t>"05/01/2000"</t>
   </si>
   <si>
     <t>"120"</t>
   </si>
   <si>
-    <t>"2022"</t>
-  </si>
-  <si>
-    <t>"10/Ene/1956"</t>
-  </si>
-  <si>
-    <t>"6000000"</t>
-  </si>
-  <si>
-    <t>"600000"</t>
-  </si>
-  <si>
-    <t>"Enero"</t>
-  </si>
-  <si>
-    <t>"05/01/2000"</t>
-  </si>
-  <si>
-    <t>05/01/2022</t>
-  </si>
-  <si>
-    <t>"SECRETARIA DISTRITAL DE INTEGRACIÓN SOCIAL"</t>
-  </si>
-  <si>
-    <t>"79290009"</t>
-  </si>
-  <si>
-    <t>"1.70"</t>
-  </si>
-  <si>
-    <t>"132"</t>
-  </si>
-  <si>
-    <t>"34500000"</t>
-  </si>
-  <si>
-    <t>"MIGUEL ANTONIO"</t>
-  </si>
-  <si>
-    <t>"MIGUEL"</t>
-  </si>
-  <si>
-    <t>"ANTONIO"</t>
-  </si>
-  <si>
-    <t>"TORRES"</t>
-  </si>
-  <si>
-    <t>"AMAYA"</t>
-  </si>
-  <si>
-    <t>"22/Feb/2022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pagaduria</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cedula</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Plazo </t>
-  </si>
-  <si>
-    <t>montoSolicitado</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DiasHabilesIntereses </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ingresos  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> descLey  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> descNomina </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mes      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaDesembolso </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> primerNombre </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> segundoNombre </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> primerApellido </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> segundoApellido </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaActual   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> oficinaAsesor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Actividad    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TotalActivos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vlrCompasSaneamientos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TipoContrato </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FechaIngreso </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Celular      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> departamento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ciudad      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rutaPDF                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DestinoCredito     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> genero </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EstadoCivil </t>
-  </si>
-  <si>
-    <t>direccionResidencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TipoVivienda </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PapellidoReferencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PnombreReferencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TelefonoResidencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TelefonoTrabajo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Codigo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AnoAnalisis </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TipoDesen  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Banco                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AccountingSource   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AccountingName                                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FechaRegistro </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cartera1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Saneamiento2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Credito </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nombresApellidos           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaNacimiento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Contacto                </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lineaCredito                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estadoActual </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> page </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> codigo  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaExpedicion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estrado     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> claseVivienda </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> posicionHogar   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nivelEscolaridad </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cuotaHipotecaria </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoDocNomina            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> otrosIngresos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> modalidadDesembolso      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoCliente </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> paisNacimiento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lugarDeNacimiento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nacionalidad </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> profesion   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mesesResidencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> numeroHijos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> personasACargo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoPension </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> codigoProgramaNomina </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaTerminacion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nitAfiliacion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoDocumento           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cargo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nombreBeneficario    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> documentoBeneficiario </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> celularBeneficiario </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> monedaExtranjera </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoTransanccion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> productoBancario </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> banco       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> numProducto </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoProducto         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pais       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ciudadExt </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> monto  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> moneda  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> funcionarioPublico </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> recursosPublicos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> expuestoPoliticamente </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaExpuesto </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mes       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fecha        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AnnoAfetacion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaActual  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Banco                                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vinculo     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> plan     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tomarSeguroAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nombresSeguroAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> parentescoSeguroAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pNombreRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sNombreRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pApellidoRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sApellidoRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> relacionRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> celRefP       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pNombreRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sNombreRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pApellidoRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sApellidoRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> relacionRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> celRefF      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> decisionExcepcion </t>
-  </si>
-  <si>
-    <t>"Soacha"</t>
-  </si>
-  <si>
-    <t>"Soltera/o"</t>
-  </si>
-  <si>
-    <t>"Arriendo"</t>
-  </si>
-  <si>
-    <t>"ALEYDA RODRIGUEZ GONZALEZ"</t>
-  </si>
-  <si>
-    <t>"15/02/1956"</t>
-  </si>
-  <si>
-    <t>"Entidad donde trabaja"</t>
-  </si>
-  <si>
-    <t>"Libre inversion"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"06/08/1976" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Estrato 1" </t>
-  </si>
-  <si>
-    <t>"Casa"</t>
-  </si>
-  <si>
-    <t>"Jefe de hogar"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Universitario" </t>
-  </si>
-  <si>
-    <t>"100000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Desprendible de nómina" </t>
-  </si>
-  <si>
-    <t>"5000000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Pago masivo (efectivo)" </t>
-  </si>
-  <si>
-    <t>"AAA"</t>
-  </si>
-  <si>
-    <t>"colombia"</t>
-  </si>
-  <si>
-    <t>"colombiano"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"ingeniero" </t>
-  </si>
-  <si>
-    <t>"24"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"2"   </t>
-  </si>
-  <si>
-    <t>"pension"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"123456"  </t>
-  </si>
-  <si>
-    <t>"30/12/2022"</t>
-  </si>
-  <si>
-    <t>"123456"</t>
-  </si>
-  <si>
-    <t>"Certificación laboral"</t>
-  </si>
-  <si>
-    <t>"CEO"</t>
-  </si>
-  <si>
-    <t>"Luis Perez Ramirez"</t>
-  </si>
-  <si>
-    <t>"1234567890"</t>
-  </si>
-  <si>
-    <t>"3183903022"</t>
-  </si>
-  <si>
-    <t>"No"</t>
-  </si>
-  <si>
-    <t>"Importaciones"</t>
-  </si>
-  <si>
-    <t>"Santander"</t>
-  </si>
-  <si>
-    <t>"966855"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Inversiones en oro" </t>
-  </si>
-  <si>
-    <t>"Alemania"</t>
-  </si>
-  <si>
-    <t>"Berlin"</t>
-  </si>
-  <si>
-    <t>"8500"</t>
-  </si>
-  <si>
-    <t>"Euros"</t>
-  </si>
-  <si>
-    <t>"12/12/2008"</t>
-  </si>
-  <si>
-    <t>"Febrero"</t>
-  </si>
-  <si>
-    <t>"20/07/1963"</t>
-  </si>
-  <si>
-    <t>"16/02/2022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t>"Vinculado"</t>
-  </si>
-  <si>
-    <t>"Plan 1"</t>
-  </si>
-  <si>
-    <t>"Si"</t>
-  </si>
-  <si>
-    <t>"Juli Macias"</t>
-  </si>
-  <si>
-    <t>"Prima"</t>
-  </si>
-  <si>
-    <t>"maria"</t>
-  </si>
-  <si>
-    <t>"camila"</t>
-  </si>
-  <si>
-    <t>"lopez"</t>
-  </si>
-  <si>
-    <t>"cardenas"</t>
-  </si>
-  <si>
-    <t>"Amigo"</t>
-  </si>
-  <si>
-    <t>"3204567894"</t>
-  </si>
-  <si>
-    <t>"juan"</t>
-  </si>
-  <si>
-    <t>"david"</t>
-  </si>
-  <si>
-    <t>"reyes"</t>
-  </si>
-  <si>
-    <t>"sanchez"</t>
-  </si>
-  <si>
-    <t>"Hijo"</t>
-  </si>
-  <si>
-    <t>"3204047804"</t>
-  </si>
-  <si>
-    <t>NumRadicacion</t>
-  </si>
-  <si>
-    <t>"92840"</t>
-  </si>
-  <si>
-    <t>tipocontratoAbacus</t>
-  </si>
-  <si>
-    <t>"Pensionado por Invalidez"</t>
-  </si>
-  <si>
-    <t>"02/Marzo/2022"</t>
-  </si>
-  <si>
-    <t>29/10/2022</t>
-  </si>
-  <si>
-    <t>"05/05/2022"</t>
-  </si>
-  <si>
-    <t>"7349400"</t>
-  </si>
-  <si>
-    <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
+    <t>"80000000"</t>
+  </si>
+  <si>
+    <t>"1.71"</t>
   </si>
 </sst>
 </file>
@@ -5353,8 +5368,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,19 +5459,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>21</v>
@@ -5465,7 +5480,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -5510,210 +5525,210 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH1" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>88</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>91</v>
-      </c>
       <c r="AR1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="K2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" t="s">
+        <v>320</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="R2" t="s">
+        <v>330</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>327</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR2" t="s">
         <v>93</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AT1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" t="s">
-        <v>126</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="R2" t="s">
-        <v>145</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AT2" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="AU2" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="AV2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX2" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU2" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="AW2" s="2">
-        <v>90537</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5850,13 +5865,13 @@
         <v>19</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>21</v>
@@ -5880,228 +5895,228 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>82</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>83</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>84</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>85</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>86</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>87</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>88</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="AM1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AR1" t="s">
         <v>92</v>
       </c>
-      <c r="AR1" t="s">
-        <v>93</v>
-      </c>
       <c r="AS1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT1" t="s">
         <v>63</v>
       </c>
-      <c r="AT1" t="s">
-        <v>64</v>
-      </c>
       <c r="AU1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AV1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AY1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="R2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y2" t="s">
         <v>119</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Z2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="S2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" t="s">
-        <v>96</v>
-      </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>48</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>50</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>51</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI2" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>54</v>
       </c>
-      <c r="AI2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>55</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AL2" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="AM2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP2" t="s">
         <v>60</v>
       </c>
-      <c r="AN2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>77</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AR2" t="s">
         <v>61</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AS2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AR2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AU2" s="10" t="s">
-        <v>79</v>
-      </c>
       <c r="AV2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="AW2" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AX2" s="7" t="s">
+      <c r="AY2" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -6124,8 +6139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:DN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6183,714 +6198,714 @@
   <sheetData>
     <row r="1" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" t="s">
+        <v>143</v>
+      </c>
+      <c r="P1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>145</v>
+      </c>
+      <c r="R1" t="s">
         <v>146</v>
       </c>
-      <c r="B1" t="s">
+      <c r="S1" t="s">
         <v>147</v>
       </c>
-      <c r="C1" t="s">
+      <c r="T1" t="s">
         <v>148</v>
       </c>
-      <c r="D1" t="s">
+      <c r="U1" t="s">
         <v>149</v>
       </c>
-      <c r="E1" t="s">
+      <c r="V1" t="s">
         <v>150</v>
-      </c>
-      <c r="F1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" t="s">
-        <v>154</v>
-      </c>
-      <c r="J1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" t="s">
-        <v>156</v>
-      </c>
-      <c r="L1" t="s">
-        <v>157</v>
-      </c>
-      <c r="M1" t="s">
-        <v>158</v>
-      </c>
-      <c r="N1" t="s">
-        <v>159</v>
-      </c>
-      <c r="O1" t="s">
-        <v>160</v>
-      </c>
-      <c r="P1" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>162</v>
-      </c>
-      <c r="R1" t="s">
-        <v>163</v>
-      </c>
-      <c r="S1" t="s">
-        <v>164</v>
-      </c>
-      <c r="T1" t="s">
-        <v>165</v>
-      </c>
-      <c r="U1" t="s">
-        <v>166</v>
-      </c>
-      <c r="V1" t="s">
-        <v>167</v>
       </c>
       <c r="W1" t="s">
         <v>3</v>
       </c>
       <c r="X1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AO1" t="s">
         <v>168</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AP1" t="s">
         <v>169</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AQ1" t="s">
         <v>170</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AR1" t="s">
         <v>171</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AS1" t="s">
         <v>172</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AT1" t="s">
         <v>173</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AU1" t="s">
         <v>174</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AV1" t="s">
         <v>175</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AW1" t="s">
         <v>176</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AX1" t="s">
         <v>177</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AY1" t="s">
         <v>178</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AZ1" t="s">
         <v>179</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="BA1" t="s">
         <v>180</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BB1" t="s">
         <v>181</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BC1" t="s">
         <v>182</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BD1" t="s">
         <v>183</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BE1" t="s">
         <v>184</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BF1" t="s">
         <v>185</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BG1" t="s">
         <v>186</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BH1" t="s">
         <v>187</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BI1" t="s">
         <v>188</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BJ1" t="s">
         <v>189</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BK1" t="s">
         <v>190</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BL1" t="s">
         <v>191</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BM1" t="s">
         <v>192</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BN1" t="s">
         <v>193</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BO1" t="s">
         <v>194</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BP1" t="s">
         <v>195</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BQ1" t="s">
         <v>196</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BR1" t="s">
         <v>197</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BS1" t="s">
         <v>198</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BT1" t="s">
         <v>199</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BU1" t="s">
         <v>200</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BV1" t="s">
         <v>201</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BW1" t="s">
         <v>202</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BX1" t="s">
         <v>203</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BY1" t="s">
         <v>204</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BZ1" t="s">
         <v>205</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="CA1" t="s">
         <v>206</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="CB1" t="s">
         <v>207</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="CC1" t="s">
         <v>208</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="CD1" t="s">
         <v>209</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="CE1" t="s">
         <v>210</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="CF1" t="s">
         <v>211</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="CG1" t="s">
         <v>212</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CH1" t="s">
         <v>213</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="CI1" t="s">
         <v>214</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CJ1" t="s">
         <v>215</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CK1" t="s">
         <v>216</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CL1" t="s">
         <v>217</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CM1" t="s">
         <v>218</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CN1" t="s">
         <v>219</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CO1" t="s">
         <v>220</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CP1" t="s">
         <v>221</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CQ1" t="s">
         <v>222</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CR1" t="s">
         <v>223</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CS1" t="s">
         <v>224</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CT1" t="s">
         <v>225</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CU1" t="s">
         <v>226</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CV1" t="s">
         <v>227</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CW1" t="s">
         <v>228</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CX1" t="s">
         <v>229</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CY1" t="s">
         <v>230</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CZ1" t="s">
         <v>231</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="DA1" t="s">
         <v>232</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="DB1" t="s">
         <v>233</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="DC1" t="s">
         <v>234</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="DD1" t="s">
         <v>235</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="DE1" t="s">
         <v>236</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="DF1" t="s">
         <v>237</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="DG1" t="s">
         <v>238</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="DH1" t="s">
         <v>239</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="DI1" t="s">
         <v>240</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DJ1" t="s">
         <v>241</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DK1" t="s">
         <v>242</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DL1" t="s">
         <v>243</v>
       </c>
-      <c r="CV1" t="s">
-        <v>244</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>245</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>246</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>247</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>248</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>249</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>250</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>251</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>252</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>253</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>254</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>255</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>256</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>257</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>258</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>259</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>260</v>
-      </c>
       <c r="DM1" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="DN1" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K2" t="s">
+        <v>312</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="O2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="AO2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>247</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>249</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>250</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>251</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>252</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>253</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>255</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>257</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>258</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>259</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>260</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>264</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>265</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>46</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>266</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>267</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>268</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>269</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>270</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>271</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>273</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>274</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>276</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>277</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>278</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>279</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>280</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>281</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>282</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>283</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>284</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>285</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>286</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>126</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>287</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>288</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>289</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>290</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>291</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>292</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>293</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>294</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>295</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>296</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>297</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>298</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>299</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>300</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>301</v>
+      </c>
+      <c r="DH2" t="s">
         <v>302</v>
       </c>
-      <c r="K2" t="s">
-        <v>329</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="P2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>263</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN2" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="AO2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AQ2" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>264</v>
-      </c>
-      <c r="AV2" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>266</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>267</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>96</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>123</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>268</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>269</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>270</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>271</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>272</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>273</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>274</v>
-      </c>
-      <c r="BI2" t="s">
+      <c r="DI2" t="s">
+        <v>303</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>304</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>305</v>
+      </c>
+      <c r="DL2" t="s">
         <v>275</v>
       </c>
-      <c r="BJ2" t="s">
-        <v>276</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>277</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>278</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>278</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>279</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>280</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>281</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>282</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>47</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>283</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>284</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>285</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>286</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>287</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>288</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>289</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>290</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>291</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>292</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>293</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>292</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>294</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>295</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>296</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>297</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>298</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>299</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>300</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>292</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>292</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>292</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>301</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>302</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>303</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>128</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>304</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>305</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>306</v>
-      </c>
-      <c r="CV2" t="s">
+      <c r="DM2" t="s">
         <v>307</v>
       </c>
-      <c r="CW2" t="s">
-        <v>308</v>
-      </c>
-      <c r="CX2" t="s">
+      <c r="DN2" t="s">
         <v>309</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>310</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>311</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>312</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>313</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>314</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>315</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>316</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>317</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>318</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>319</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>320</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>321</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>322</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>292</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>324</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste pesp y firma documentos codigo ado digicredito
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788BC6D0-6192-4D83-B06F-28C15F33A806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE3CAC2-A909-428B-ADE1-2B97A715EA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -2574,7 +2574,7 @@
     <author>Analista Desarrollo59</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{14EC37F8-B1CE-482C-91B1-03735921E8DC}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{02B788F3-AF89-4242-90F1-5E84EBA7D9AB}">
       <text>
         <r>
           <rPr>
@@ -2598,7 +2598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{F9E8595A-23BA-4DB3-B46E-01018F1FA409}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{5EF34D1E-6B8D-4A88-ABB4-FACDE88F7539}">
       <text>
         <r>
           <rPr>
@@ -2623,7 +2623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{55A53080-C1FB-40D6-A441-13CD31AFDCE5}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{6FEEF052-3112-4D62-8A91-27B5E63792DD}">
       <text>
         <r>
           <rPr>
@@ -2650,7 +2650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{69FE05B5-F12F-4829-8DDB-42C97E3E1EA8}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{587E5A27-C9D0-4E14-90B6-9688121D8803}">
       <text>
         <r>
           <rPr>
@@ -2675,7 +2675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{C69CA3F5-DBD0-4CC6-A0AD-CBFE67BB8EEB}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{93113BA2-014F-4DB7-B5A5-C907911F5406}">
       <text>
         <r>
           <rPr>
@@ -2700,7 +2700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{3F4CCB1D-50CE-480D-9EC0-A6817C6F24F9}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{5B128BE1-BBE7-4527-8AC2-3A6E00A5E14A}">
       <text>
         <r>
           <rPr>
@@ -2724,7 +2724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{E454EBB3-EC80-485E-8ED0-E14D9DB199E6}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{A27344A4-46D1-4DB0-831E-5DC75AD798BE}">
       <text>
         <r>
           <rPr>
@@ -2749,7 +2749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{0B32431B-38A0-411A-A33E-EE806A4DEA7D}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{0A6CAF21-AFEA-4363-B9AD-16A49D2E85C2}">
       <text>
         <r>
           <rPr>
@@ -2774,7 +2774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{FA1D7BE3-3B7F-4DCA-A4CE-BFD83D83DB02}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{42042A6B-621F-4281-A476-C86309A379C7}">
       <text>
         <r>
           <rPr>
@@ -2799,7 +2799,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{32A1FAA3-720F-496E-9580-85EAF9357829}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{C78D135F-9FE9-47CD-B9ED-CE3F35CB54FA}">
       <text>
         <r>
           <rPr>
@@ -2825,7 +2825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{6D03E615-84E8-4E68-8D53-2A506A82F15B}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{5702296B-8380-4570-9E06-EB5FF35D24A1}">
       <text>
         <r>
           <rPr>
@@ -2854,7 +2854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{7BBB61E6-D414-4208-B894-8498E90E6BF4}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{9B055CE4-E1B1-425B-8C6C-96E649456119}">
       <text>
         <r>
           <rPr>
@@ -2879,7 +2879,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{2A7DB574-2680-4F42-AA17-0273ED1652C5}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{E9F72C29-DBEB-4F17-A4E5-BD750D8B494E}">
       <text>
         <r>
           <rPr>
@@ -2904,7 +2904,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{35E3954E-27F5-4D8E-B5AE-2D92996B7CE3}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{7A4750C0-7D55-46CD-ADF0-B82E04142181}">
       <text>
         <r>
           <rPr>
@@ -2929,7 +2929,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{20BC2F34-9EB3-4DDE-AB8C-D9C818E510C5}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{D27A31ED-49F8-4AAE-AC57-EB0604A5C7CA}">
       <text>
         <r>
           <rPr>
@@ -2954,7 +2954,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{28E6406B-75DE-4929-884A-6A1D0DE34633}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{FB09C25E-4931-4FB9-BFDB-BF524B56FD69}">
       <text>
         <r>
           <rPr>
@@ -2982,7 +2982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{C446B284-3F79-416C-AF3A-9B8871C2AFDE}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{2704F02D-A83F-4155-A759-47C8BFCDE43E}">
       <text>
         <r>
           <rPr>
@@ -3007,7 +3007,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{A7757CBD-9E84-430F-8DC3-CDFEDDFCE724}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{6B3AE9B1-09A3-481D-AA7A-5E18CB9E48AE}">
       <text>
         <r>
           <rPr>
@@ -3033,7 +3033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{A0A984DB-EFCD-4EB0-AD27-77A82B4F56B4}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{AECE4650-7E0B-484B-AFD1-C07EDD53A59F}">
       <text>
         <r>
           <rPr>
@@ -3058,7 +3058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{EBDFA775-CADD-43A0-9CCD-D5C9028C271D}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{71B3E1A7-01E6-4016-B37A-10CEAE905CFF}">
       <text>
         <r>
           <rPr>
@@ -3083,7 +3083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{8C9E7585-560E-4420-9EBE-3B97C6653B4F}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{30CE1681-E2F2-44CC-83B5-94DEF9336FF9}">
       <text>
         <r>
           <rPr>
@@ -3108,7 +3108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{31837F90-3CD5-4B90-B6F2-CBA49035EA25}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{A71E8BA2-B048-41C2-B73F-05C30E86494F}">
       <text>
         <r>
           <rPr>
@@ -3136,7 +3136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{D4D53531-DC1E-4991-A944-EF9D12182BA5}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{D9B8AD38-0562-465F-AEBD-107D3F77346C}">
       <text>
         <r>
           <rPr>
@@ -3161,7 +3161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{3964D7D7-D3BF-4469-85CA-CA0F700EB0E2}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{22CB6F5C-C690-4085-A485-401429A4C392}">
       <text>
         <r>
           <rPr>
@@ -3186,7 +3186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{D4CC3540-85F5-4050-A403-EEF8F25EA707}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{81551ADD-BE8F-4AE6-B3AD-108244F2091D}">
       <text>
         <r>
           <rPr>
@@ -3210,7 +3210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{06A14CA3-47E2-47BB-BD32-9903BAF2CB6D}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{36210278-1C48-4469-A7CF-5E35B019A666}">
       <text>
         <r>
           <rPr>
@@ -3234,7 +3234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{E97F49C8-820A-467F-9547-76B2E1939AA0}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{3BDDEACB-3C74-46D6-AE9C-C145022AB073}">
       <text>
         <r>
           <rPr>
@@ -3259,7 +3259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{F0BC3096-6C97-4D4F-8AEC-42244F2A9649}">
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{33BC859C-199C-4B8B-BB48-6FFCBA5DCFA9}">
       <text>
         <r>
           <rPr>
@@ -3283,7 +3283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{2EA7BF7F-A12D-45FB-9D2E-145C04B70564}">
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{15221440-2BBD-419E-88DF-4C397DA11173}">
       <text>
         <r>
           <rPr>
@@ -3310,7 +3310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{F0D0575B-FDEC-42F6-BED2-E89711FCF0A7}">
+    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{D530F630-AF47-4E87-A1A3-678DBED4025C}">
       <text>
         <r>
           <rPr>
@@ -3335,7 +3335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{01551780-738D-4966-AB01-08FB90C0B242}">
+    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{70749C47-8831-4FB2-9DED-A1B5D2116B63}">
       <text>
         <r>
           <rPr>
@@ -3360,7 +3360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{50F40B8A-6A4B-4FEC-A5A3-F1079E220339}">
+    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{00E3137F-3A2A-4A03-B83A-35C958B3F29E}">
       <text>
         <r>
           <rPr>
@@ -3387,7 +3387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{5406339D-E896-4C6B-A6B2-0132B4229850}">
+    <comment ref="AG2" authorId="0" shapeId="0" xr:uid="{BC9715F9-3794-4B2F-93BB-A8A47DBD360D}">
       <text>
         <r>
           <rPr>
@@ -3413,7 +3413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{DF12E362-0153-468B-8645-D3CEC67A88A0}">
+    <comment ref="AH2" authorId="0" shapeId="0" xr:uid="{D0553B1A-72EA-4588-A0D9-1A9A7664BFEB}">
       <text>
         <r>
           <rPr>
@@ -3439,7 +3439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{58FB3D71-988A-4D3D-9B24-0BEE0868F88E}">
+    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{08D83E90-2F9A-422B-BAF4-5DD28132E32F}">
       <text>
         <r>
           <rPr>
@@ -3465,7 +3465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{EDA8B302-4223-45EE-B80C-E61652C1E467}">
+    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{852348E2-98A8-4D68-80EB-3E6CDD48F7A8}">
       <text>
         <r>
           <rPr>
@@ -3491,7 +3491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK2" authorId="0" shapeId="0" xr:uid="{80E78FEC-E9CF-4B3D-B074-0B3A0A348E11}">
+    <comment ref="AK2" authorId="0" shapeId="0" xr:uid="{3928E8A7-85CD-4288-BFEB-F6478779E52C}">
       <text>
         <r>
           <rPr>
@@ -3515,7 +3515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL2" authorId="0" shapeId="0" xr:uid="{6ABE95F5-B956-43C6-AB3A-A5FECDCD5EDB}">
+    <comment ref="AL2" authorId="0" shapeId="0" xr:uid="{A6CBB220-0C35-46A9-AAD3-F5FFC0184154}">
       <text>
         <r>
           <rPr>
@@ -3541,7 +3541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM2" authorId="0" shapeId="0" xr:uid="{3C4F35CB-15B9-4498-9D25-7F823334B549}">
+    <comment ref="AM2" authorId="0" shapeId="0" xr:uid="{A821F306-CA06-4E12-ADE2-F5018E2F3CC7}">
       <text>
         <r>
           <rPr>
@@ -3566,7 +3566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN2" authorId="0" shapeId="0" xr:uid="{BC7AB2E0-EEA5-4836-A618-950FC472CB40}">
+    <comment ref="AN2" authorId="0" shapeId="0" xr:uid="{0DEB6CD7-6A6F-4233-9E0F-FD170FEF89DB}">
       <text>
         <r>
           <rPr>
@@ -3590,7 +3590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO2" authorId="0" shapeId="0" xr:uid="{8A525466-AD2C-4F9A-89D9-0570F5942A8B}">
+    <comment ref="AO2" authorId="0" shapeId="0" xr:uid="{D2FA0C65-F2CF-4037-8BC2-D9696D8E13B3}">
       <text>
         <r>
           <rPr>
@@ -3614,7 +3614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP2" authorId="0" shapeId="0" xr:uid="{F3A92176-49D5-4586-968C-24AD737B34E3}">
+    <comment ref="AP2" authorId="0" shapeId="0" xr:uid="{5AF45776-197C-42CB-B21C-7AE470CD6B9B}">
       <text>
         <r>
           <rPr>
@@ -3638,7 +3638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ2" authorId="0" shapeId="0" xr:uid="{BDF5EE0A-1411-49FA-88D0-E9F89805BFA5}">
+    <comment ref="AQ2" authorId="0" shapeId="0" xr:uid="{68C6A5B3-B6AF-464B-8E51-B6A667C8B39A}">
       <text>
         <r>
           <rPr>
@@ -3668,7 +3668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR2" authorId="0" shapeId="0" xr:uid="{3C68A674-3190-4C9C-956C-8BF61409D6D1}">
+    <comment ref="AR2" authorId="0" shapeId="0" xr:uid="{1CF2B5F9-CE3B-4472-88C4-8047702C4EEE}">
       <text>
         <r>
           <rPr>
@@ -3693,7 +3693,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS2" authorId="0" shapeId="0" xr:uid="{0B412B49-E1E5-4894-9B26-17FDD4693346}">
+    <comment ref="AS2" authorId="0" shapeId="0" xr:uid="{48C939C2-64D9-4182-837D-1E9A8EC91E7E}">
       <text>
         <r>
           <rPr>
@@ -3723,7 +3723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="336">
   <si>
     <t>Cedula</t>
   </si>
@@ -3836,12 +3836,6 @@
     <t>"ARBOLEDA"</t>
   </si>
   <si>
-    <t>"prueba123@gmail.com"</t>
-  </si>
-  <si>
-    <t>"3125127717"</t>
-  </si>
-  <si>
     <t>"Cundinamarca"</t>
   </si>
   <si>
@@ -3857,9 +3851,6 @@
     <t>"xx"</t>
   </si>
   <si>
-    <t>"COLFONDOS"</t>
-  </si>
-  <si>
     <t>"17/Mar/1956"</t>
   </si>
   <si>
@@ -4046,694 +4037,700 @@
     <t>NumRadicadoCredito</t>
   </si>
   <si>
-    <t>"ALEYDA"</t>
-  </si>
-  <si>
     <t>"Jubilados"</t>
   </si>
   <si>
-    <t>"86313"</t>
-  </si>
-  <si>
-    <t>"52912399"</t>
-  </si>
-  <si>
-    <t>"RODRIGUEZ"</t>
-  </si>
-  <si>
-    <t>"GONZALEZ"</t>
-  </si>
-  <si>
-    <t>"50"</t>
+    <t>"300000"</t>
+  </si>
+  <si>
+    <t>"200000"</t>
+  </si>
+  <si>
+    <t>"1030000"</t>
+  </si>
+  <si>
+    <t>"3125117718"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"prueba321@gmail.com" </t>
+  </si>
+  <si>
+    <t>"3125127718"</t>
+  </si>
+  <si>
+    <t>"12345"</t>
+  </si>
+  <si>
+    <t>"1.80"</t>
+  </si>
+  <si>
+    <t>"Educación propia"</t>
+  </si>
+  <si>
+    <t>"05/01/2022"</t>
+  </si>
+  <si>
+    <t>"2022"</t>
+  </si>
+  <si>
+    <t>"Enero"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pagaduria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cedula</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plazo </t>
+  </si>
+  <si>
+    <t>montoSolicitado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DiasHabilesIntereses </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingresos  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> descLey  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> descNomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mes      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaDesembolso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> primerNombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> segundoNombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> primerApellido </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> segundoApellido </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaActual   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oficinaAsesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Actividad    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TotalActivos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vlrCompasSaneamientos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoContrato </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FechaIngreso </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Celular      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> departamento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciudad      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rutaPDF                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DestinoCredito     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genero </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EstadoCivil </t>
+  </si>
+  <si>
+    <t>direccionResidencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoVivienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PapellidoReferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PnombreReferencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TelefonoResidencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TelefonoTrabajo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Codigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnoAnalisis </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TipoDesen  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banco                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AccountingSource   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AccountingName                                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FechaRegistro </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartera1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saneamiento2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Credito </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombresApellidos           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contacto                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lineaCredito                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estadoActual </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> page </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> codigo  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaExpedicion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> estrado     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> claseVivienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> posicionHogar   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nivelEscolaridad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cuotaHipotecaria </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoDocNomina            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> otrosIngresos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> modalidadDesembolso      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoCliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> paisNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lugarDeNacimiento </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nacionalidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> profesion   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mesesResidencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numeroHijos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> personasACargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoPension </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> codigoProgramaNomina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaTerminacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nitAfiliacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoDocumento           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombreBeneficario    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> documentoBeneficiario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celularBeneficiario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> monedaExtranjera </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoTransanccion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> productoBancario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> banco       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numProducto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tipoProducto         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pais       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ciudadExt </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> monto  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> moneda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> funcionarioPublico </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recursosPublicos </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> expuestoPoliticamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaExpuesto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mes       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fecha        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AnnoAfetacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fechaActual  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banco                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vinculo     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> plan     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tomarSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombresSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> parentescoSeguroAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pNombreRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sNombreRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pApellidoRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sApellidoRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relacionRefP </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celRefP       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pNombreRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sNombreRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pApellidoRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sApellidoRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> relacionRefF </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celRefF      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> decisionExcepcion </t>
+  </si>
+  <si>
+    <t>"Soacha"</t>
+  </si>
+  <si>
+    <t>"Soltera/o"</t>
+  </si>
+  <si>
+    <t>"Arriendo"</t>
+  </si>
+  <si>
+    <t>"Entidad donde trabaja"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"06/08/1976" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Estrato 1" </t>
+  </si>
+  <si>
+    <t>"Casa"</t>
+  </si>
+  <si>
+    <t>"Jefe de hogar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Universitario" </t>
+  </si>
+  <si>
+    <t>"100000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Desprendible de nómina" </t>
+  </si>
+  <si>
+    <t>"5000000"</t>
+  </si>
+  <si>
+    <t>"AAA"</t>
+  </si>
+  <si>
+    <t>"colombia"</t>
+  </si>
+  <si>
+    <t>"colombiano"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ingeniero" </t>
+  </si>
+  <si>
+    <t>"24"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"2"   </t>
+  </si>
+  <si>
+    <t>"pension"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"123456"  </t>
+  </si>
+  <si>
+    <t>"30/12/2022"</t>
+  </si>
+  <si>
+    <t>"123456"</t>
+  </si>
+  <si>
+    <t>"Certificación laboral"</t>
+  </si>
+  <si>
+    <t>"CEO"</t>
+  </si>
+  <si>
+    <t>"Luis Perez Ramirez"</t>
+  </si>
+  <si>
+    <t>"1234567890"</t>
+  </si>
+  <si>
+    <t>"3183903022"</t>
+  </si>
+  <si>
+    <t>"No"</t>
+  </si>
+  <si>
+    <t>"Importaciones"</t>
+  </si>
+  <si>
+    <t>"Santander"</t>
+  </si>
+  <si>
+    <t>"966855"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Inversiones en oro" </t>
+  </si>
+  <si>
+    <t>"Alemania"</t>
+  </si>
+  <si>
+    <t>"Berlin"</t>
+  </si>
+  <si>
+    <t>"8500"</t>
+  </si>
+  <si>
+    <t>"Euros"</t>
+  </si>
+  <si>
+    <t>"12/12/2008"</t>
+  </si>
+  <si>
+    <t>"Febrero"</t>
+  </si>
+  <si>
+    <t>"20/07/1963"</t>
+  </si>
+  <si>
+    <t>"16/02/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t>"Vinculado"</t>
+  </si>
+  <si>
+    <t>"Plan 1"</t>
+  </si>
+  <si>
+    <t>"Juli Macias"</t>
+  </si>
+  <si>
+    <t>"Prima"</t>
+  </si>
+  <si>
+    <t>"maria"</t>
+  </si>
+  <si>
+    <t>"camila"</t>
+  </si>
+  <si>
+    <t>"lopez"</t>
+  </si>
+  <si>
+    <t>"cardenas"</t>
+  </si>
+  <si>
+    <t>"Amigo"</t>
+  </si>
+  <si>
+    <t>"3204567894"</t>
+  </si>
+  <si>
+    <t>"juan"</t>
+  </si>
+  <si>
+    <t>"david"</t>
+  </si>
+  <si>
+    <t>"reyes"</t>
+  </si>
+  <si>
+    <t>"sanchez"</t>
+  </si>
+  <si>
+    <t>"Hijo"</t>
+  </si>
+  <si>
+    <t>"3204047804"</t>
+  </si>
+  <si>
+    <t>NumRadicacion</t>
+  </si>
+  <si>
+    <t>tipocontratoAbacus</t>
+  </si>
+  <si>
+    <t>"Pensionado por Invalidez"</t>
+  </si>
+  <si>
+    <t>"P.A COLPENSIONES"</t>
+  </si>
+  <si>
+    <t>"51618664"</t>
+  </si>
+  <si>
+    <t>"10"</t>
+  </si>
+  <si>
+    <t>"6500000"</t>
+  </si>
+  <si>
+    <t>"350000"</t>
+  </si>
+  <si>
+    <t>"28/02/2022"</t>
+  </si>
+  <si>
+    <t>"OLGA"</t>
+  </si>
+  <si>
+    <t>"BEATRIZ"</t>
+  </si>
+  <si>
+    <t>"CONTRERAS"</t>
+  </si>
+  <si>
+    <t>"DE CAMACHO"</t>
+  </si>
+  <si>
+    <t>"2000001"</t>
+  </si>
+  <si>
+    <t>"prueba321@gmail.com"</t>
+  </si>
+  <si>
+    <t>"alejando"</t>
+  </si>
+  <si>
+    <t>"'ACRED','EGRESO'"</t>
+  </si>
+  <si>
+    <t>"upper('Desembolso egreso'),upper('Desembolso activación de crédito')"</t>
+  </si>
+  <si>
+    <t>"7/3/2022"</t>
+  </si>
+  <si>
+    <t>"20/Jun/1958"</t>
+  </si>
+  <si>
+    <t>"Cartagena"</t>
+  </si>
+  <si>
+    <t>"05/01/2000"</t>
+  </si>
+  <si>
+    <t>"120"</t>
+  </si>
+  <si>
+    <t>"80000000"</t>
+  </si>
+  <si>
+    <t>"1.71"</t>
+  </si>
+  <si>
+    <t>"Marzo"</t>
+  </si>
+  <si>
+    <t>"14/03/2022"</t>
+  </si>
+  <si>
+    <t>"81768"</t>
+  </si>
+  <si>
+    <t>"18/Mar/2022"</t>
+  </si>
+  <si>
+    <t>"Compra de cartera"</t>
+  </si>
+  <si>
+    <t>"3994518"</t>
+  </si>
+  <si>
+    <t>"1.70"</t>
+  </si>
+  <si>
+    <t>"16"</t>
+  </si>
+  <si>
+    <t>"50500000"</t>
+  </si>
+  <si>
+    <t>"8500000"</t>
   </si>
   <si>
     <t>"250000"</t>
   </si>
   <si>
-    <t>"8500000"</t>
-  </si>
-  <si>
-    <t>"300000"</t>
-  </si>
-  <si>
-    <t>"200000"</t>
-  </si>
-  <si>
-    <t>"1030000"</t>
-  </si>
-  <si>
-    <t>"3125117718"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"prueba321@gmail.com" </t>
-  </si>
-  <si>
-    <t>"3125127718"</t>
-  </si>
-  <si>
-    <t>"12345"</t>
-  </si>
-  <si>
-    <t>"1.80"</t>
-  </si>
-  <si>
-    <t>"Educación propia"</t>
-  </si>
-  <si>
-    <t>"05/01/2022"</t>
-  </si>
-  <si>
-    <t>"2022"</t>
-  </si>
-  <si>
-    <t>"Enero"</t>
-  </si>
-  <si>
-    <t>"1.70"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pagaduria</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cedula</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Plazo </t>
-  </si>
-  <si>
-    <t>montoSolicitado</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DiasHabilesIntereses </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ingresos  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> descLey  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> descNomina </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mes      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaDesembolso </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> primerNombre </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> segundoNombre </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> primerApellido </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> segundoApellido </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaActual   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> oficinaAsesor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Actividad    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TotalActivos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vlrCompasSaneamientos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TipoContrato </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FechaIngreso </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Celular      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> departamento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ciudad      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rutaPDF                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DestinoCredito     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> genero </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EstadoCivil </t>
-  </si>
-  <si>
-    <t>direccionResidencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TipoVivienda </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PapellidoReferencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PnombreReferencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TelefonoResidencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TelefonoTrabajo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Codigo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AnoAnalisis </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TipoDesen  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Banco                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AccountingSource   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AccountingName                                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FechaRegistro </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cartera1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Saneamiento2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Credito </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nombresApellidos           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaNacimiento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Contacto                </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lineaCredito                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estadoActual </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> page </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> codigo  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaExpedicion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estrado     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> claseVivienda </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> posicionHogar   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nivelEscolaridad </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cuotaHipotecaria </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoDocNomina            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> otrosIngresos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> modalidadDesembolso      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoCliente </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> paisNacimiento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lugarDeNacimiento </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nacionalidad </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> profesion   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mesesResidencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> numeroHijos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> personasACargo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoPension </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> codigoProgramaNomina </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaTerminacion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nitAfiliacion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoDocumento           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cargo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nombreBeneficario    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> documentoBeneficiario </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> celularBeneficiario </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> monedaExtranjera </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoTransanccion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> productoBancario </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> banco       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> numProducto </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tipoProducto         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pais       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ciudadExt </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> monto  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> moneda  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> funcionarioPublico </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> recursosPublicos </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> expuestoPoliticamente </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaExpuesto </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mes       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fecha        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AnnoAfetacion </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fechaActual  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Banco                                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vinculo     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> plan     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tomarSeguroAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nombresSeguroAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> parentescoSeguroAP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pNombreRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sNombreRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pApellidoRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sApellidoRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> relacionRefP </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> celRefP       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pNombreRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sNombreRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pApellidoRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sApellidoRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> relacionRefF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> celRefF      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> decisionExcepcion </t>
-  </si>
-  <si>
-    <t>"Soacha"</t>
-  </si>
-  <si>
-    <t>"Soltera/o"</t>
-  </si>
-  <si>
-    <t>"Arriendo"</t>
-  </si>
-  <si>
-    <t>"ALEYDA RODRIGUEZ GONZALEZ"</t>
+    <t>"SERGIO"</t>
+  </si>
+  <si>
+    <t>"SEGUNDO"</t>
+  </si>
+  <si>
+    <t>"URZOLA"</t>
+  </si>
+  <si>
+    <t>"BERTEL"</t>
+  </si>
+  <si>
+    <t>"500000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"lespitiameza@gmail.com" </t>
+  </si>
+  <si>
+    <t>"3219176522"</t>
+  </si>
+  <si>
+    <t>"DELIO ARNULFO ROJAS GUIO"</t>
   </si>
   <si>
     <t>"15/02/1956"</t>
   </si>
   <si>
-    <t>"Entidad donde trabaja"</t>
-  </si>
-  <si>
-    <t>"Libre inversion"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"06/08/1976" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Estrato 1" </t>
-  </si>
-  <si>
-    <t>"Casa"</t>
-  </si>
-  <si>
-    <t>"Jefe de hogar"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Universitario" </t>
-  </si>
-  <si>
-    <t>"100000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Desprendible de nómina" </t>
-  </si>
-  <si>
-    <t>"5000000"</t>
-  </si>
-  <si>
     <t xml:space="preserve">"Pago masivo (efectivo)" </t>
   </si>
   <si>
-    <t>"AAA"</t>
-  </si>
-  <si>
-    <t>"colombia"</t>
-  </si>
-  <si>
-    <t>"colombiano"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"ingeniero" </t>
-  </si>
-  <si>
-    <t>"24"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"2"   </t>
-  </si>
-  <si>
-    <t>"pension"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"123456"  </t>
-  </si>
-  <si>
-    <t>"30/12/2022"</t>
-  </si>
-  <si>
-    <t>"123456"</t>
-  </si>
-  <si>
-    <t>"Certificación laboral"</t>
-  </si>
-  <si>
-    <t>"CEO"</t>
-  </si>
-  <si>
-    <t>"Luis Perez Ramirez"</t>
-  </si>
-  <si>
-    <t>"1234567890"</t>
-  </si>
-  <si>
-    <t>"3183903022"</t>
-  </si>
-  <si>
-    <t>"No"</t>
-  </si>
-  <si>
-    <t>"Importaciones"</t>
-  </si>
-  <si>
-    <t>"Santander"</t>
-  </si>
-  <si>
-    <t>"966855"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Inversiones en oro" </t>
-  </si>
-  <si>
-    <t>"Alemania"</t>
-  </si>
-  <si>
-    <t>"Berlin"</t>
-  </si>
-  <si>
-    <t>"8500"</t>
-  </si>
-  <si>
-    <t>"Euros"</t>
-  </si>
-  <si>
-    <t>"12/12/2008"</t>
-  </si>
-  <si>
-    <t>"Febrero"</t>
-  </si>
-  <si>
-    <t>"20/07/1963"</t>
-  </si>
-  <si>
-    <t>"16/02/2022"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t>"Vinculado"</t>
-  </si>
-  <si>
-    <t>"Plan 1"</t>
-  </si>
-  <si>
-    <t>"Si"</t>
-  </si>
-  <si>
-    <t>"Juli Macias"</t>
-  </si>
-  <si>
-    <t>"Prima"</t>
-  </si>
-  <si>
-    <t>"maria"</t>
-  </si>
-  <si>
-    <t>"camila"</t>
-  </si>
-  <si>
-    <t>"lopez"</t>
-  </si>
-  <si>
-    <t>"cardenas"</t>
-  </si>
-  <si>
-    <t>"Amigo"</t>
-  </si>
-  <si>
-    <t>"3204567894"</t>
-  </si>
-  <si>
-    <t>"juan"</t>
-  </si>
-  <si>
-    <t>"david"</t>
-  </si>
-  <si>
-    <t>"reyes"</t>
-  </si>
-  <si>
-    <t>"sanchez"</t>
-  </si>
-  <si>
-    <t>"Hijo"</t>
-  </si>
-  <si>
-    <t>"3204047804"</t>
-  </si>
-  <si>
-    <t>NumRadicacion</t>
-  </si>
-  <si>
-    <t>"92840"</t>
-  </si>
-  <si>
-    <t>tipocontratoAbacus</t>
-  </si>
-  <si>
-    <t>"Pensionado por Invalidez"</t>
-  </si>
-  <si>
-    <t>"02/Marzo/2022"</t>
-  </si>
-  <si>
-    <t>29/10/2022</t>
-  </si>
-  <si>
-    <t>"05/05/2022"</t>
-  </si>
-  <si>
-    <t>"7349400"</t>
-  </si>
-  <si>
-    <t>"Bancolombia Remanentes - 60237038927 - REMANENTE"</t>
-  </si>
-  <si>
-    <t>"P.A COLPENSIONES"</t>
-  </si>
-  <si>
-    <t>"51618664"</t>
-  </si>
-  <si>
-    <t>"10"</t>
-  </si>
-  <si>
-    <t>"6500000"</t>
-  </si>
-  <si>
-    <t>"350000"</t>
-  </si>
-  <si>
-    <t>"28/02/2022"</t>
-  </si>
-  <si>
-    <t>"OLGA"</t>
-  </si>
-  <si>
-    <t>"BEATRIZ"</t>
-  </si>
-  <si>
-    <t>"CONTRERAS"</t>
-  </si>
-  <si>
-    <t>"DE CAMACHO"</t>
-  </si>
-  <si>
-    <t>"2000001"</t>
-  </si>
-  <si>
-    <t>"prueba321@gmail.com"</t>
-  </si>
-  <si>
-    <t>"alejando"</t>
-  </si>
-  <si>
-    <t>"'ACRED','EGRESO'"</t>
-  </si>
-  <si>
-    <t>"upper('Desembolso egreso'),upper('Desembolso activación de crédito')"</t>
-  </si>
-  <si>
-    <t>"7/3/2022"</t>
-  </si>
-  <si>
-    <t>"20/Jun/1958"</t>
-  </si>
-  <si>
-    <t>"Cartagena"</t>
-  </si>
-  <si>
-    <t>"05/01/2000"</t>
-  </si>
-  <si>
-    <t>"120"</t>
-  </si>
-  <si>
-    <t>"80000000"</t>
-  </si>
-  <si>
-    <t>"1.71"</t>
+    <t>"92865"</t>
   </si>
 </sst>
 </file>
@@ -4826,7 +4823,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4861,6 +4858,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4868,7 +4866,227 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5368,7 +5586,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -5459,19 +5677,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>21</v>
@@ -5480,7 +5698,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -5525,129 +5743,129 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>80</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>81</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>82</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>83</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>84</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>85</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>86</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>87</v>
       </c>
-      <c r="AO1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>89</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>92</v>
-      </c>
       <c r="AS1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AT1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AU1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="D2" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="L2" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="R2" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>31</v>
@@ -5656,87 +5874,87 @@
         <v>32</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="AC2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="AG2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="AH2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK2" t="s">
         <v>48</v>
       </c>
-      <c r="AI2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>50</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
+        <v>304</v>
+      </c>
+      <c r="AN2" t="s">
         <v>51</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AO2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AM2" t="s">
-        <v>327</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AP2" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="AR2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AS2" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AT2" s="11" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="AU2" s="11" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:C2 E2:XFD2">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="AA2" r:id="rId1" display="prueba321@gmail.com" xr:uid="{68C5CA67-349F-451E-87B3-1675F58DE642}"/>
@@ -5865,13 +6083,13 @@
         <v>19</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>21</v>
@@ -5895,129 +6113,129 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AR1" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>92</v>
-      </c>
       <c r="AS1" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AT1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AU1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY1" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AX1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="O2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
         <v>43</v>
-      </c>
-      <c r="P2" t="s">
-        <v>46</v>
       </c>
       <c r="Q2" t="s">
         <v>32</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="S2" t="s">
         <v>34</v>
@@ -6026,7 +6244,7 @@
         <v>34</v>
       </c>
       <c r="U2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="V2" t="s">
         <v>35</v>
@@ -6035,96 +6253,96 @@
         <v>36</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="Y2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="Z2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AA2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO2" t="s">
         <v>73</v>
       </c>
-      <c r="AB2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS2" t="s">
         <v>76</v>
       </c>
-      <c r="AP2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AR2" t="s">
+      <c r="AT2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AS2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT2" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="AU2" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AV2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW2" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="AW2" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="AX2" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:XFD1048576 A1:AU2 AZ1:XFD2">
-    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AY2">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="X2" r:id="rId1" display="dabogado@excelcredit.co" xr:uid="{0565F543-D6A3-457F-A02B-20E7DC298B68}"/>
@@ -6139,8 +6357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26F554-6D5A-43B1-9BC4-58521368D054}">
   <dimension ref="A1:DN2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="DM6" sqref="DM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6198,411 +6416,411 @@
   <sheetData>
     <row r="1" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" t="s">
+      <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="C1" t="s">
+      <c r="O1" t="s">
         <v>131</v>
       </c>
-      <c r="D1" t="s">
+      <c r="P1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" t="s">
         <v>134</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>135</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>137</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>138</v>
-      </c>
-      <c r="K1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" t="s">
-        <v>141</v>
-      </c>
-      <c r="N1" t="s">
-        <v>142</v>
-      </c>
-      <c r="O1" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R1" t="s">
-        <v>146</v>
-      </c>
-      <c r="S1" t="s">
-        <v>147</v>
-      </c>
-      <c r="T1" t="s">
-        <v>148</v>
-      </c>
-      <c r="U1" t="s">
-        <v>149</v>
-      </c>
-      <c r="V1" t="s">
-        <v>150</v>
       </c>
       <c r="W1" t="s">
         <v>3</v>
       </c>
       <c r="X1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>151</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AK1" t="s">
         <v>152</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AL1" t="s">
         <v>153</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AM1" t="s">
         <v>154</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AN1" t="s">
         <v>155</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AO1" t="s">
         <v>156</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AP1" t="s">
         <v>157</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AQ1" t="s">
         <v>158</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AR1" t="s">
         <v>159</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AS1" t="s">
         <v>160</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AT1" t="s">
         <v>161</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AU1" t="s">
         <v>162</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AV1" t="s">
         <v>163</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AW1" t="s">
         <v>164</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AX1" t="s">
         <v>165</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AY1" t="s">
         <v>166</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AZ1" t="s">
         <v>167</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BA1" t="s">
         <v>168</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BB1" t="s">
         <v>169</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BC1" t="s">
         <v>170</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BD1" t="s">
         <v>171</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BE1" t="s">
         <v>172</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BF1" t="s">
         <v>173</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BG1" t="s">
         <v>174</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BH1" t="s">
         <v>175</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BI1" t="s">
         <v>176</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BJ1" t="s">
         <v>177</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BK1" t="s">
         <v>178</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BL1" t="s">
         <v>179</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BM1" t="s">
         <v>180</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BN1" t="s">
         <v>181</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BO1" t="s">
         <v>182</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BP1" t="s">
         <v>183</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BQ1" t="s">
         <v>184</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BR1" t="s">
         <v>185</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BS1" t="s">
         <v>186</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BT1" t="s">
         <v>187</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BU1" t="s">
         <v>188</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BV1" t="s">
         <v>189</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BW1" t="s">
         <v>190</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BX1" t="s">
         <v>191</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BY1" t="s">
         <v>192</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BZ1" t="s">
         <v>193</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="CA1" t="s">
         <v>194</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="CB1" t="s">
         <v>195</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CC1" t="s">
         <v>196</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="CD1" t="s">
         <v>197</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CE1" t="s">
         <v>198</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CF1" t="s">
         <v>199</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CG1" t="s">
         <v>200</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CH1" t="s">
         <v>201</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CI1" t="s">
         <v>202</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CJ1" t="s">
         <v>203</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CK1" t="s">
         <v>204</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CL1" t="s">
         <v>205</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CM1" t="s">
         <v>206</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CN1" t="s">
         <v>207</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CO1" t="s">
         <v>208</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CP1" t="s">
         <v>209</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CQ1" t="s">
         <v>210</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CR1" t="s">
         <v>211</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CS1" t="s">
         <v>212</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CT1" t="s">
         <v>213</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CU1" t="s">
         <v>214</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CV1" t="s">
         <v>215</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CW1" t="s">
         <v>216</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CX1" t="s">
         <v>217</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CY1" t="s">
         <v>218</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CZ1" t="s">
         <v>219</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="DA1" t="s">
         <v>220</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="DB1" t="s">
         <v>221</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="DC1" t="s">
         <v>222</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="DD1" t="s">
         <v>223</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DE1" t="s">
         <v>224</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DF1" t="s">
         <v>225</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DG1" t="s">
         <v>226</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DH1" t="s">
         <v>227</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DI1" t="s">
         <v>228</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DJ1" t="s">
         <v>229</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DK1" t="s">
         <v>230</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DL1" t="s">
         <v>231</v>
       </c>
-      <c r="DA1" t="s">
-        <v>232</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>233</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>234</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>235</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>236</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>237</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>238</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>239</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>240</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>241</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>242</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>243</v>
-      </c>
       <c r="DM1" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="DN1" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>292</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>110</v>
+        <v>319</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>113</v>
+        <v>321</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>115</v>
+        <v>323</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>114</v>
+        <v>324</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>285</v>
+        <v>314</v>
       </c>
       <c r="K2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>107</v>
+        <v>325</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>95</v>
+        <v>326</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>111</v>
+        <v>327</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>112</v>
+        <v>328</v>
       </c>
       <c r="P2" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="R2" s="14" t="s">
         <v>28</v>
@@ -6611,360 +6829,366 @@
         <v>30</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>46</v>
+        <v>329</v>
       </c>
       <c r="U2" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="V2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="Z2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>41</v>
-      </c>
       <c r="AB2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE2" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>316</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>318</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>237</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>239</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>241</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>243</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>334</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>244</v>
+      </c>
+      <c r="BL2" t="s">
         <v>245</v>
       </c>
-      <c r="AE2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="BM2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BN2" t="s">
         <v>246</v>
       </c>
-      <c r="AG2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN2" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="AO2" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ2" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU2" t="s">
+      <c r="BO2" t="s">
         <v>247</v>
       </c>
-      <c r="AV2" s="15" t="s">
+      <c r="BP2" t="s">
         <v>248</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BQ2" t="s">
         <v>249</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BR2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BS2" t="s">
         <v>250</v>
       </c>
-      <c r="AY2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>122</v>
-      </c>
-      <c r="BB2" t="s">
+      <c r="BT2" t="s">
         <v>251</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BU2" t="s">
         <v>252</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BV2" t="s">
         <v>253</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BW2" t="s">
         <v>254</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BX2" t="s">
         <v>255</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BY2" t="s">
         <v>256</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BZ2" t="s">
         <v>257</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="CA2" t="s">
         <v>258</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="CB2" t="s">
         <v>259</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="CC2" t="s">
         <v>260</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="CD2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CE2" t="s">
         <v>261</v>
       </c>
-      <c r="BM2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BN2" t="s">
+      <c r="CF2" t="s">
         <v>262</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="CG2" t="s">
         <v>263</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="CH2" t="s">
         <v>264</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="CI2" t="s">
         <v>265</v>
       </c>
-      <c r="BR2" t="s">
-        <v>46</v>
-      </c>
-      <c r="BS2" t="s">
+      <c r="CJ2" t="s">
         <v>266</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="CK2" t="s">
         <v>267</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="CL2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CO2" t="s">
         <v>268</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="CP2" t="s">
         <v>269</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="CQ2" t="s">
         <v>270</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="CR2" t="s">
+        <v>115</v>
+      </c>
+      <c r="CS2" t="s">
         <v>271</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CT2" t="s">
         <v>272</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CU2" t="s">
         <v>273</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CV2" t="s">
         <v>274</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CW2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CX2" t="s">
         <v>275</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CY2" t="s">
         <v>276</v>
       </c>
-      <c r="CD2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CE2" t="s">
+      <c r="CZ2" t="s">
         <v>277</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="DA2" t="s">
         <v>278</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="DB2" t="s">
         <v>279</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="DC2" t="s">
         <v>280</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="DD2" t="s">
         <v>281</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="DE2" t="s">
         <v>282</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="DF2" t="s">
         <v>283</v>
       </c>
-      <c r="CL2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CO2" t="s">
+      <c r="DG2" t="s">
         <v>284</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="DH2" t="s">
         <v>285</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="DI2" t="s">
         <v>286</v>
       </c>
-      <c r="CR2" t="s">
-        <v>126</v>
-      </c>
-      <c r="CS2" t="s">
+      <c r="DJ2" t="s">
         <v>287</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="DK2" t="s">
         <v>288</v>
       </c>
-      <c r="CU2" t="s">
-        <v>289</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>290</v>
-      </c>
-      <c r="CW2" t="s">
+      <c r="DL2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>335</v>
+      </c>
+      <c r="DN2" t="s">
         <v>291</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>292</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>293</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>294</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>295</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>296</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>297</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>298</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>299</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>300</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>301</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>302</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>303</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>304</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>305</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>275</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>307</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>309</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="CU2:XFD2 CB2 BY2 A1:XFD1">
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="duplicateValues" dxfId="39" priority="77"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CU2:DL2 CB2 BY2 DN2:XFD2">
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
+  <conditionalFormatting sqref="B2">
     <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="C2:G2">
     <cfRule type="duplicateValues" dxfId="15" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:G2">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H2:K2">
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N2">
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:P2">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:T2">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:V2">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:AB2">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:AB2">
+  <conditionalFormatting sqref="AC2:AE2">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AE2">
+  <conditionalFormatting sqref="AF2:AG2">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF2:AG2">
+  <conditionalFormatting sqref="AH2:AL2">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AL2">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AM2">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN2">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO2:AP2">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2">
+  <conditionalFormatting sqref="AR2:AS2">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR2:AS2">
+  <conditionalFormatting sqref="DM2">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="W2" r:id="rId1" display="prueba321@gmail.com" xr:uid="{0827CE73-83FA-4AC6-B5E7-8249E9A9C693}"/>
+    <hyperlink ref="W2" r:id="rId1" display="prueba123@gmail.com" xr:uid="{ADDD52C1-F874-4CFD-8BA3-E5A833CBBBFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Mejoras proceso captura de pantallas Originación - allure
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788BC6D0-6192-4D83-B06F-28C15F33A806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F64040-613D-4C65-BD7B-546A39AABAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{06BED893-92A4-4214-B78F-5DEA0D3E11C8}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="10" r:id="rId1"/>
@@ -1780,28 +1780,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{C4B08A73-B2D5-49C8-89DB-D6C79B1E3FF8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Analista Desarrollo59:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Primer nombre del Cliente;
-*Completo en mayuscula</t>
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{AA9B1B28-F7BE-40D8-8412-9DA54417DAD9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Analista Desarrollo59:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nombre del Credito;
+*Se recomienda usar el primer nombre del Cliente</t>
         </r>
       </text>
     </comment>
@@ -2413,7 +2413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT2" authorId="0" shapeId="0" xr:uid="{73F9885D-1388-4F5F-823B-FA5B788FFD95}">
+    <comment ref="AT2" authorId="0" shapeId="0" xr:uid="{DB56D02E-2099-41E6-BDF1-01B3DBE69F37}">
       <text>
         <r>
           <rPr>
@@ -3723,7 +3723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="325">
   <si>
     <t>Cedula</t>
   </si>
@@ -3806,9 +3806,6 @@
     <t>FechaServidor</t>
   </si>
   <si>
-    <t>"9777757"</t>
-  </si>
-  <si>
     <t>"Pensionado"</t>
   </si>
   <si>
@@ -3827,15 +3824,6 @@
     <t>"10/03/2000"</t>
   </si>
   <si>
-    <t>"CARLOS"</t>
-  </si>
-  <si>
-    <t>"HERRERA"</t>
-  </si>
-  <si>
-    <t>"ARBOLEDA"</t>
-  </si>
-  <si>
     <t>"prueba123@gmail.com"</t>
   </si>
   <si>
@@ -3860,9 +3848,6 @@
     <t>"COLFONDOS"</t>
   </si>
   <si>
-    <t>"17/Mar/1956"</t>
-  </si>
-  <si>
     <t>"0"</t>
   </si>
   <si>
@@ -3905,9 +3890,6 @@
     <t>"Noviembre"</t>
   </si>
   <si>
-    <t>"2021"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "Efectivo" </t>
   </si>
   <si>
@@ -3917,12 +3899,6 @@
     <t>Banco</t>
   </si>
   <si>
-    <t>"Remanentes - 60237038927 - REMANENTE"</t>
-  </si>
-  <si>
-    <t>"ALCALDIA MUNICIPAL DE MANIZALES NÓMINA JUBILADOS"</t>
-  </si>
-  <si>
     <t>"Bogotá Centro"</t>
   </si>
   <si>
@@ -3953,18 +3929,9 @@
     <t>Saneamiento2</t>
   </si>
   <si>
-    <t>"830000"</t>
-  </si>
-  <si>
-    <t>"19/10/2021"</t>
-  </si>
-  <si>
     <t>"8300538122 -  FIDEICOMISO SOLUCIONES"</t>
   </si>
   <si>
-    <t>"19/Oct/2021"</t>
-  </si>
-  <si>
     <t>DestinoCredito</t>
   </si>
   <si>
@@ -4034,9 +4001,6 @@
     <t xml:space="preserve">"'ACRED','EGRESO'" </t>
   </si>
   <si>
-    <t>29/10/2021</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -4082,21 +4046,12 @@
     <t>"1030000"</t>
   </si>
   <si>
-    <t>"3125117718"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"prueba321@gmail.com" </t>
-  </si>
-  <si>
     <t>"3125127718"</t>
   </si>
   <si>
     <t>"12345"</t>
   </si>
   <si>
-    <t>"1.80"</t>
-  </si>
-  <si>
     <t>"Educación propia"</t>
   </si>
   <si>
@@ -4700,9 +4655,6 @@
     <t>"DE CAMACHO"</t>
   </si>
   <si>
-    <t>"2000001"</t>
-  </si>
-  <si>
     <t>"prueba321@gmail.com"</t>
   </si>
   <si>
@@ -4733,7 +4685,19 @@
     <t>"80000000"</t>
   </si>
   <si>
-    <t>"1.71"</t>
+    <t>24/03/2022</t>
+  </si>
+  <si>
+    <t>"24/03/2022"</t>
+  </si>
+  <si>
+    <t>"31/03/2022"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"aalvarezv99@gmail.com" </t>
+  </si>
+  <si>
+    <t>"1230000"</t>
   </si>
 </sst>
 </file>
@@ -4868,7 +4832,17 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5368,8 +5342,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="AL1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5459,19 +5433,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>21</v>
@@ -5480,7 +5454,7 @@
         <v>22</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>5</v>
@@ -5525,218 +5499,218 @@
         <v>26</v>
       </c>
       <c r="AG1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="AH1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" t="s">
         <v>81</v>
       </c>
-      <c r="AI1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AS1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AV1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AR1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="R2" t="s">
+        <v>314</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="T2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="K2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="R2" t="s">
-        <v>330</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="W2" s="12" t="s">
+      <c r="AA2" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH2" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL2" t="s">
         <v>48</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
+        <v>311</v>
+      </c>
+      <c r="AN2" t="s">
         <v>49</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AO2" t="s">
         <v>50</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AP2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AL2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>327</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AP2" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="AR2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="AS2" s="10" t="s">
-        <v>64</v>
+        <v>299</v>
       </c>
       <c r="AT2" s="11" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="AU2" s="11" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A3:XFD1048576 A2:C2 E2:XFD2">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="AA2" r:id="rId1" display="prueba321@gmail.com" xr:uid="{68C5CA67-349F-451E-87B3-1675F58DE642}"/>
@@ -5751,8 +5725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC7558A-6DD3-4212-BAB4-0FE9FA09F3EE}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AO9" sqref="AO9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,13 +5839,13 @@
         <v>19</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>21</v>
@@ -5895,235 +5869,238 @@
         <v>25</v>
       </c>
       <c r="AC1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AR1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH1" t="s">
+      <c r="AS1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU1" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AX1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AY1" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AX1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" t="s">
+        <v>95</v>
+      </c>
+      <c r="U2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" t="s">
+        <v>99</v>
+      </c>
+      <c r="W2" t="s">
+        <v>100</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="AB2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="AG2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>324</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>322</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>321</v>
+      </c>
+      <c r="AT2" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="AU2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>118</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="S2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" t="s">
-        <v>95</v>
-      </c>
-      <c r="V2" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AU2" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="AV2" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="AW2" s="11" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="AX2" s="7" t="s">
-        <v>103</v>
+        <v>320</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:XFD1048576 A1:AU2 AZ1:XFD2">
-    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
+  <conditionalFormatting sqref="A3:XFD1048576 AZ1:XFD2 A1:AU1 AU2 A2:AS2">
+    <cfRule type="duplicateValues" dxfId="20" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV1:AY2">
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT2">
     <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -6198,714 +6175,714 @@
   <sheetData>
     <row r="1" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" t="s">
+      <c r="Q1" t="s">
         <v>130</v>
       </c>
-      <c r="C1" t="s">
+      <c r="R1" t="s">
         <v>131</v>
       </c>
-      <c r="D1" t="s">
+      <c r="S1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" t="s">
+      <c r="T1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" t="s">
+      <c r="U1" t="s">
         <v>134</v>
       </c>
-      <c r="G1" t="s">
+      <c r="V1" t="s">
         <v>135</v>
-      </c>
-      <c r="H1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" t="s">
-        <v>141</v>
-      </c>
-      <c r="N1" t="s">
-        <v>142</v>
-      </c>
-      <c r="O1" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R1" t="s">
-        <v>146</v>
-      </c>
-      <c r="S1" t="s">
-        <v>147</v>
-      </c>
-      <c r="T1" t="s">
-        <v>148</v>
-      </c>
-      <c r="U1" t="s">
-        <v>149</v>
-      </c>
-      <c r="V1" t="s">
-        <v>150</v>
       </c>
       <c r="W1" t="s">
         <v>3</v>
       </c>
       <c r="X1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM1" t="s">
         <v>151</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AN1" t="s">
         <v>152</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AO1" t="s">
         <v>153</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AP1" t="s">
         <v>154</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AQ1" t="s">
         <v>155</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AR1" t="s">
         <v>156</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AS1" t="s">
         <v>157</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AT1" t="s">
         <v>158</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AU1" t="s">
         <v>159</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AV1" t="s">
         <v>160</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AW1" t="s">
         <v>161</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AX1" t="s">
         <v>162</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AY1" t="s">
         <v>163</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AZ1" t="s">
         <v>164</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BA1" t="s">
         <v>165</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BB1" t="s">
         <v>166</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BC1" t="s">
         <v>167</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BD1" t="s">
         <v>168</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BE1" t="s">
         <v>169</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BF1" t="s">
         <v>170</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BG1" t="s">
         <v>171</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BH1" t="s">
         <v>172</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BI1" t="s">
         <v>173</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BJ1" t="s">
         <v>174</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BK1" t="s">
         <v>175</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BL1" t="s">
         <v>176</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BM1" t="s">
         <v>177</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BN1" t="s">
         <v>178</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BO1" t="s">
         <v>179</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BP1" t="s">
         <v>180</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BQ1" t="s">
         <v>181</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BR1" t="s">
         <v>182</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BS1" t="s">
         <v>183</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BT1" t="s">
         <v>184</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BU1" t="s">
         <v>185</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BV1" t="s">
         <v>186</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BW1" t="s">
         <v>187</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BX1" t="s">
         <v>188</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BY1" t="s">
         <v>189</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BZ1" t="s">
         <v>190</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="CA1" t="s">
         <v>191</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="CB1" t="s">
         <v>192</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="CC1" t="s">
         <v>193</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="CD1" t="s">
         <v>194</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="CE1" t="s">
         <v>195</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CF1" t="s">
         <v>196</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="CG1" t="s">
         <v>197</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CH1" t="s">
         <v>198</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CI1" t="s">
         <v>199</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CJ1" t="s">
         <v>200</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CK1" t="s">
         <v>201</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CL1" t="s">
         <v>202</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CM1" t="s">
         <v>203</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CN1" t="s">
         <v>204</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CO1" t="s">
         <v>205</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CP1" t="s">
         <v>206</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CQ1" t="s">
         <v>207</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CR1" t="s">
         <v>208</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CS1" t="s">
         <v>209</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CT1" t="s">
         <v>210</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CU1" t="s">
         <v>211</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CV1" t="s">
         <v>212</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CW1" t="s">
         <v>213</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CX1" t="s">
         <v>214</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CY1" t="s">
         <v>215</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CZ1" t="s">
         <v>216</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="DA1" t="s">
         <v>217</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="DB1" t="s">
         <v>218</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="DC1" t="s">
         <v>219</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="DD1" t="s">
         <v>220</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="DE1" t="s">
         <v>221</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="DF1" t="s">
         <v>222</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="DG1" t="s">
         <v>223</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DH1" t="s">
         <v>224</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DI1" t="s">
         <v>225</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DJ1" t="s">
         <v>226</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DK1" t="s">
         <v>227</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DL1" t="s">
         <v>228</v>
       </c>
-      <c r="CX1" t="s">
-        <v>229</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>230</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>231</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>232</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>233</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>234</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>235</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>236</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>237</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>238</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>239</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>240</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>241</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>242</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>243</v>
-      </c>
       <c r="DM1" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="DN1" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="J2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="AO2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>237</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>238</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>239</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>241</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>243</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>244</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>247</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>251</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>252</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>253</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>255</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>257</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>261</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>262</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>263</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>264</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>265</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>266</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>267</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>268</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>269</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>270</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>271</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>111</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>272</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>273</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>274</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>275</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>276</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>277</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>278</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>280</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>281</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>282</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>283</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>284</v>
+      </c>
+      <c r="DF2" t="s">
         <v>285</v>
       </c>
-      <c r="K2" t="s">
-        <v>312</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="P2" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>246</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN2" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="AO2" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AP2" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ2" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>247</v>
-      </c>
-      <c r="AV2" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>249</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>250</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>122</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>251</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>252</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>253</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>254</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>255</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>256</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>257</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>258</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>259</v>
-      </c>
-      <c r="BK2" t="s">
+      <c r="DG2" t="s">
+        <v>286</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>287</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>288</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>289</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>290</v>
+      </c>
+      <c r="DL2" t="s">
         <v>260</v>
       </c>
-      <c r="BL2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>262</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>263</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>264</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>265</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>46</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>266</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>267</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>268</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>269</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>270</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>271</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>272</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>273</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>274</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>276</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>277</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>278</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>279</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>280</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>281</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>282</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>283</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>275</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>284</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>285</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>286</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>126</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>287</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>288</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>289</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>290</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>291</v>
-      </c>
-      <c r="CX2" t="s">
+      <c r="DM2" t="s">
         <v>292</v>
       </c>
-      <c r="CY2" t="s">
-        <v>293</v>
-      </c>
-      <c r="CZ2" t="s">
+      <c r="DN2" t="s">
         <v>294</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>295</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>296</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>297</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>298</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>299</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>300</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>301</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>302</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>303</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>304</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>305</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>275</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>307</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste pesp y firma documentos codigo ado digicredit
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataOriginacion.xlsx
+++ b/src/test/resources/Data/AutomationDataOriginacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\analista.pruebas6\Documents\TestAutomationPOM\TestAutomationPOM\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB831382-3704-4128-AD0D-5A4A05FB11EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB242A1D-0912-4913-8ED2-ED5D9E89B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="1875" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OriginacionCredito" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nombre de la pagaduría, debe estar escrita tal cual en Base de datos</t>
         </r>
@@ -74,7 +74,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cedula del cliente
 *No debe contener puntos ni comas</t>
@@ -99,7 +99,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Año de nacimiento del cliente;
 *Debe estar en formato:
@@ -127,7 +127,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tasa del Credito;
 *Debe siempre estar a dos decimales.
@@ -154,7 +154,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Plazo en meses del crédito
 </t>
@@ -179,7 +179,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Monto solicitado para el crédito;
 *No debe tener puntos ni comas</t>
@@ -204,7 +204,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Días hábiles de intereses iniciales</t>
         </r>
@@ -228,7 +228,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ingresos del cliente;
 *Debe estar sin puntos ni comas</t>
@@ -253,7 +253,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Descuentos de Ley;
 *Sin puntos ni comas</t>
@@ -278,7 +278,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Descuento de nomina;
 *Sin puntos ni comas</t>
@@ -303,7 +303,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Mes en el cual se va a lanzar la Originación;
 *Siempre mes Actual
@@ -329,7 +329,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Fecha en la cual se hará el desembolso del Crédito;
 *Formato de fecha:
@@ -358,7 +358,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nombre del Crédito;
 *Se recomienda usar el primer nombre del Cliente</t>
@@ -383,7 +383,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nombre del Crédito;
 *Se recomienda usar el primer nombre del Cliente</t>
@@ -408,7 +408,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Segundo nombre del Cliente;
 *Completo en mayúscula</t>
@@ -433,7 +433,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer Apellido del Cliente;
 *Completo en mayúscula</t>
@@ -458,7 +458,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Segundo Apellido del Cliente;
 *Completo en mayúscula</t>
@@ -483,7 +483,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha Actual
 *Formato de fecha:
@@ -511,7 +511,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Oficina en que se solicita el crédito;
 *Debe estar escrita tal cual en base de datos</t>
@@ -536,7 +536,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Actividad del Cliente;
 *Debe ser una de las opciones disponibles en base de datos
@@ -562,7 +562,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Total suma de activos del Cliente;
 *No debe contener ni puntos ni comas</t>
@@ -587,7 +587,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valor total por la suma de las compras y saneamientos que se le van a recoger al cliente;
 *Sin puntos ni comas</t>
@@ -612,7 +612,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Revisar este campo</t>
         </r>
@@ -636,7 +636,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Colchón;
 Formato;
@@ -662,7 +662,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tipo de contrato del Cliente;
 *Tal cual en base de datos</t>
@@ -687,7 +687,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha en la que el Cliente inicio el tipo de contrato;
 *Formato de Fecha;
@@ -715,7 +715,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Correo electrónico del Cliente;
 *Para pruebas automatizadas cambiar el correo desde bases de datos por uno de prueba</t>
@@ -740,7 +740,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero Celular del Cliente;
 *Para pruebas automatizadas cambiar el celular desde bases de datos por uno de prueba</t>
@@ -765,7 +765,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Departamento en que reside el Cliente</t>
         </r>
@@ -789,7 +789,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ciudad en que reside el Cliente</t>
         </r>
@@ -813,7 +813,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ruta o Path en la cual se almacena el PDF para pruebas de carga de documentos;
 *Verificar su existencia antes de lanzar una prueba</t>
@@ -838,7 +838,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Revisar este campo</t>
         </r>
@@ -862,7 +862,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Destino que se le dará al crédito solicitado</t>
         </r>
@@ -886,7 +886,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Genero del Cliente;
 *Formato, una sola letra;
@@ -913,7 +913,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Estado civil del Cliente;
 *Según las opciones del sistema</t>
@@ -938,7 +938,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dirección de residencia del Cliente;
 *Formato: Libre</t>
@@ -963,7 +963,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tipo de vivienda en la que habita el solicitante;
 *Formato;
@@ -990,7 +990,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer Apellido de la referencia del solicitante.
 *Formato;
@@ -1016,7 +1016,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer nombre de la referencia del solicitante.
 *Formato;
@@ -1042,7 +1042,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero telefónico fijo de la referencia del solicitante.
 *Formato;
@@ -1068,7 +1068,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero telefónico de la referencia del solicitante.
 *Formato;
@@ -1094,7 +1094,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -1118,7 +1118,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Año actual.
 *Formato;
@@ -1144,7 +1144,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tipo de desembolso del crédito.
 *Debe coincidir con las opciones del sistema</t>
@@ -1169,7 +1169,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -1193,7 +1193,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -1217,7 +1217,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -1241,7 +1241,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha en la cual se genera el registro del Cliente.
 Fecha Actual
@@ -1271,7 +1271,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero de radicación de la solicitud.
 Consultarlo en base de datos.</t>
@@ -1296,7 +1296,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero de radicación del Crédito
 Consultarlo en base de datos.</t>
@@ -1331,7 +1331,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nombre de la pagaduria, debe estar escrita tal cual en Base de datos</t>
         </r>
@@ -1355,7 +1355,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Cedula del cliente
 *No debe tener puntos ni comas</t>
@@ -1380,7 +1380,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Año de nacimiento del cliente;
 *Debe estar en formato:
@@ -1409,7 +1409,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Oficina en que se solicita el credito;
 *Debe estar escrita tal cual en base de datos</t>
@@ -1434,7 +1434,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Actividad del Cliente;
 *Debe ser una de las opciones diponibles en base de datos
@@ -1460,7 +1460,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tasa del Credito;
 *Debe siempre estar a dos decimales.
@@ -1487,7 +1487,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Plazo en meses del credito</t>
         </r>
@@ -1511,7 +1511,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Monto solicitado para el credito;
 *No debe tener puntos ni comas</t>
@@ -1536,7 +1536,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dias habiles de intereses iniciales</t>
         </r>
@@ -1560,7 +1560,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ingresos del cliente;
 *Debe estar sin puntos ni comas</t>
@@ -1585,7 +1585,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Descuento de nomina;
 *Sin puntos ni comas</t>
@@ -1610,7 +1610,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Total suma de activos del Cliente;
 *No debe contener ni puntos ni comas</t>
@@ -1635,7 +1635,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valor total por la suma de las compras y saneamientos que se le van a recoger al cliente;
 *Sin puntos ni comas</t>
@@ -1660,7 +1660,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Revisar este campo</t>
         </r>
@@ -1684,7 +1684,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Colchon;
 Formato;
@@ -1710,7 +1710,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tipo de contrato del Cliente;
 *Tal cual en base de datos
@@ -1736,7 +1736,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha en la que el Cliente inicio el tipo de contrato;
 *Formato de Fecha;
@@ -1764,7 +1764,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nombre del Credito;
 *Se recomienda usar el primer nombre del Cliente</t>
@@ -1789,7 +1789,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer nombre del Cliente;
 *Completo en mayuscula</t>
@@ -1814,7 +1814,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Segundo nombre del Cliente;
 *Completo en mayuscula</t>
@@ -1839,7 +1839,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer Apellido del Cliente;
 *Completo en mayúscula</t>
@@ -1864,7 +1864,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Segundo Apellido del Cliente;
 *Completo en mayúscula</t>
@@ -1889,7 +1889,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Correo electrónico del Cliente;
 *Para pruebas automatizadas cambiar el correo desde bases de datos por uno de prueba</t>
@@ -1914,7 +1914,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero Celular del Cliente;
 *Para pruebas automatizadas cambiar el celular desde bases de datos por uno de prueba</t>
@@ -1939,7 +1939,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Departamento en que reside el Cliente</t>
         </r>
@@ -1963,7 +1963,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ciudad en que reside el Cliente</t>
         </r>
@@ -1987,7 +1987,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ruta o Path en la cual se almacena el PDF para pruebas de carga de documentos;
 *Verificar su existencia antes de lanzar una prueba</t>
@@ -2012,7 +2012,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Destino que se le dará al crédito solicitado</t>
         </r>
@@ -2036,7 +2036,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Genero del Cliente;
 *Formato, una sola letra;
@@ -2063,7 +2063,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Estado civil del Cliente;
 *Según las opciones del sistema</t>
@@ -2088,7 +2088,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Dirección de residencia del Cliente;
 *Formato: Libre</t>
@@ -2113,7 +2113,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tipo de vivienda en la que habita el solicitante;
 *Formato;
@@ -2139,7 +2139,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer Apellido de la referencia del solicitante.
 *Formato;
@@ -2165,7 +2165,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Primer nombre de la referencia del solicitante.
 *Formato;
@@ -2191,7 +2191,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero telefónico fijo de la referencia del solicitante.
 *Formato;
@@ -2217,7 +2217,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero telefónico de la referencia del solicitante.
 *Formato;
@@ -2243,7 +2243,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -2267,7 +2267,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Mes en el cual se va a lanzar la Originación;
 *Siempre mes Actual
@@ -2293,7 +2293,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Monto de la primera cartera que se va a recoger;
 *No debe tener puntos ni comas</t>
@@ -2318,7 +2318,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Monto del Saneamiento que se va a recoger;
 *No debe tener puntos ni comas</t>
@@ -2343,7 +2343,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Año actual.
 *Formato;
@@ -2369,7 +2369,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tipo de desembolso del crédito.
 *Debe coincidir con las opciones del sistema</t>
@@ -2394,7 +2394,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha Actual
 *Formato de fecha:
@@ -2422,7 +2422,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar usos</t>
         </r>
@@ -2446,7 +2446,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar Usos</t>
         </r>
@@ -2470,7 +2470,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar Usos</t>
         </r>
@@ -2494,7 +2494,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Consultar Uso</t>
         </r>
@@ -2518,7 +2518,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fecha en la cual se genera el registro del Cliente.
 Fecha Actual
@@ -2548,7 +2548,7 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Numero de radicación de la solicitud.
 Consultarlo en base de datos.</t>
@@ -2560,7 +2560,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="367">
   <si>
     <t>Pagaduria</t>
   </si>
@@ -3321,357 +3321,356 @@
     <t>tipocontratoAbacus</t>
   </si>
   <si>
-    <t xml:space="preserve"> "P.A COLPENSIONES" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3994518" </t>
+    <t xml:space="preserve">"P.A COLPENSIONES" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "8500000" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"250000" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Pensionado" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"20500000"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Jubilados"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "10/03/2000" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Cundinamarca" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Anapoima" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"src/test/resources/Data/PDFPRUEBA.pdf" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Educacion propia" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "M"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Soltera/o" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Calle 2d #22-52"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Arriendo"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"perez"             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "alejandro"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "7210273"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "9007146"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3112" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2022"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "'ACRED','EGRESO'" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "upper('Desembolso egreso'), upper('Desembolso activación de crédito')" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "15/02/1956"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Entidad donde trabaja" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ""           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ""   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "12345" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "06/08/1976"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Estrato 1" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Casa"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Jefe de hogar" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Universitario"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "100000"         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Desprendible de nómina" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "5000000"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Pago masivo (efectivo)" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "AAA"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "colombia"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "colombia"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "colombiano" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ingeniero" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "24"            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2"         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "0"            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "pension"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "123456"             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "30/12/2022"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "123456"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Certificación laboral" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "CEO" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Luis Perez Ramirez" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "1234567890"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3183903022"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Importaciones"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Santander" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "966855"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Inversiones en oro" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Alemania" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Berlin"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "8500" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Euros" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "12/12/2008"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Febrero" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "20/07/1963" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2022"        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "16/02/2022" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Vinculado" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Plan 1" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Si"          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Juli Macias"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Prima"            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "maria"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "camila"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "lopez"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "cardenas"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Amigo"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3204567894" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "juan"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "david"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "reyes"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "sanchez"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Hijo"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "3204047804" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "No"              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Pensionado por Invalidez" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"14206887" </t>
   </si>
   <si>
     <t xml:space="preserve"> "1.70" </t>
   </si>
   <si>
-    <t xml:space="preserve"> "16"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "90"                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "8500000" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "250000" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "300000"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Marzo" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "14/03/2022"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "SERGIO"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "SEGUNDO"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "URZOLA"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "BERTEL"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "18/Mar/2022" </t>
+    <t xml:space="preserve">"24"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"40500000"      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"60"                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"300000"   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Marzo" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"14/03/2022"    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "JOSE"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "DEL CARMEN"     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "VILLARREAL"       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "GONZALEZ"        </t>
+  </si>
+  <si>
+    <t>"30/03/2022"</t>
   </si>
   <si>
     <t xml:space="preserve"> "Soacha"      </t>
   </si>
   <si>
-    <t xml:space="preserve"> "Pensionado" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "20500000"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "500000"              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Jubilados"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "10/03/2000" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "lespitiameza@gmail.com" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3219176522" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Cundinamarca" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Anapoima" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "src/test/resources/Data/PDFPRUEBA.pdf" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Educacion propia" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "M"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Soltera/o" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Calle 2d #22-52"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Arriendo"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "perez"             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "alejandro"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "7210273"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "9007146"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3112" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2022"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "'ACRED','EGRESO'" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "upper('Desembolso egreso'), upper('Desembolso activación de crédito')" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "0"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "0"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "81768" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "DELIO ARNULFO ROJAS GUIO" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "15/02/1956"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Entidad donde trabaja" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Compra de cartera" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ""           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ""   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "12345" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "06/08/1976"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Estrato 1" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Casa"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Jefe de hogar" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Universitario"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "100000"         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Desprendible de nómina" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "5000000"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Pago masivo (efectivo)" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "AAA"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "colombia"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "colombia"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "colombiano" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "ingeniero" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "24"            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2"         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "0"            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "pension"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "123456"             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "30/12/2022"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "123456"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Certificación laboral" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "CEO" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Luis Perez Ramirez" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "1234567890"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3183903022"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Importaciones"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Santander" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "966855"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Inversiones en oro" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Alemania" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Berlin"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "8500" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Euros" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"               </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "12/12/2008"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Febrero" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "20/07/1963" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2022"        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "16/02/2022" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Bancolombia Remanentes - 60237038927 - REMANENTE" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Vinculado" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Plan 1" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Si"          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Juli Macias"   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Prima"            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "maria"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "camila"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "lopez"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "cardenas"    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Amigo"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3204567894" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "juan"      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "david"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "reyes"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "sanchez"     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hijo"       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "3204047804" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "No"              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Pensionado por Invalidez" </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "10500000"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "92884"       </t>
+    <t xml:space="preserve">"0"              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "daabogadog@gmail.com" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"3132739036" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29/10/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"85900" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "JOSE DEL CARMEN VILLARREAL GONZALEZ" </t>
+  </si>
+  <si>
+    <t>"Libre inversion"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "92948"       </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
@@ -3705,7 +3704,20 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3728,12 +3740,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -3775,10 +3802,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Neutral" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -4993,8 +5020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DM2" sqref="DM2"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5404,370 +5431,367 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:118" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>253</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="H2" t="s">
         <v>255</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="I2" t="s">
+        <v>349</v>
+      </c>
+      <c r="J2" t="s">
+        <v>350</v>
+      </c>
+      <c r="K2" t="s">
+        <v>351</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>357</v>
+      </c>
+      <c r="R2" t="s">
         <v>256</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="S2" t="s">
+        <v>257</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="U2" t="s">
+        <v>258</v>
+      </c>
+      <c r="V2" t="s">
+        <v>259</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>267</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>269</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>271</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>272</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>273</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>274</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>275</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>276</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>361</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="AT2" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="AU2" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>277</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>278</v>
+      </c>
+      <c r="AX2" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AY2" t="s">
         <v>279</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AZ2" t="s">
         <v>280</v>
       </c>
-      <c r="AD2" s="14" t="s">
+      <c r="BA2" t="s">
         <v>281</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="BB2" t="s">
         <v>282</v>
       </c>
-      <c r="AF2" s="14" t="s">
+      <c r="BC2" t="s">
         <v>283</v>
       </c>
-      <c r="AG2" s="14" t="s">
+      <c r="BD2" t="s">
         <v>284</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="BE2" t="s">
         <v>285</v>
       </c>
-      <c r="AI2" s="14" t="s">
+      <c r="BF2" t="s">
         <v>286</v>
       </c>
-      <c r="AJ2" s="14" t="s">
+      <c r="BG2" t="s">
         <v>287</v>
       </c>
-      <c r="AK2" s="14" t="s">
+      <c r="BH2" t="s">
         <v>288</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="BI2" t="s">
         <v>289</v>
       </c>
-      <c r="AM2" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AN2" s="14" t="s">
+      <c r="BJ2" t="s">
         <v>290</v>
       </c>
-      <c r="AO2" s="14" t="s">
+      <c r="BK2" t="s">
         <v>291</v>
       </c>
-      <c r="AP2" s="14" t="s">
+      <c r="BL2" t="s">
         <v>292</v>
       </c>
-      <c r="AQ2" s="16">
-        <v>44498</v>
-      </c>
-      <c r="AR2" s="14" t="s">
+      <c r="BM2" t="s">
         <v>293</v>
       </c>
-      <c r="AS2" s="14" t="s">
+      <c r="BN2" t="s">
         <v>294</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="BO2" t="s">
         <v>295</v>
       </c>
-      <c r="AU2" s="14" t="s">
+      <c r="BP2" t="s">
         <v>296</v>
       </c>
-      <c r="AV2" s="14" t="s">
+      <c r="BQ2" t="s">
         <v>297</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="BR2" t="s">
         <v>298</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="BS2" t="s">
         <v>299</v>
       </c>
-      <c r="AY2" s="14" t="s">
+      <c r="BT2" t="s">
         <v>300</v>
       </c>
-      <c r="AZ2" s="14" t="s">
+      <c r="BU2" t="s">
         <v>301</v>
       </c>
-      <c r="BA2" s="14" t="s">
+      <c r="BV2" t="s">
         <v>302</v>
       </c>
-      <c r="BB2" s="14" t="s">
+      <c r="BW2" t="s">
         <v>303</v>
       </c>
-      <c r="BC2" s="14" t="s">
+      <c r="BX2" t="s">
         <v>304</v>
       </c>
-      <c r="BD2" s="14" t="s">
+      <c r="BY2" t="s">
         <v>305</v>
       </c>
-      <c r="BE2" s="14" t="s">
+      <c r="BZ2" t="s">
         <v>306</v>
       </c>
-      <c r="BF2" s="14" t="s">
+      <c r="CA2" t="s">
         <v>307</v>
       </c>
-      <c r="BG2" s="14" t="s">
+      <c r="CB2" t="s">
         <v>308</v>
       </c>
-      <c r="BH2" s="14" t="s">
+      <c r="CC2" t="s">
         <v>309</v>
       </c>
-      <c r="BI2" s="14" t="s">
+      <c r="CD2" t="s">
+        <v>308</v>
+      </c>
+      <c r="CE2" t="s">
         <v>310</v>
       </c>
-      <c r="BJ2" s="14" t="s">
+      <c r="CF2" t="s">
         <v>311</v>
       </c>
-      <c r="BK2" s="14" t="s">
+      <c r="CG2" t="s">
         <v>312</v>
       </c>
-      <c r="BL2" s="14" t="s">
+      <c r="CH2" t="s">
         <v>313</v>
       </c>
-      <c r="BM2" s="14" t="s">
+      <c r="CI2" t="s">
         <v>314</v>
       </c>
-      <c r="BN2" s="14" t="s">
+      <c r="CJ2" t="s">
         <v>315</v>
       </c>
-      <c r="BO2" s="14" t="s">
+      <c r="CK2" t="s">
         <v>316</v>
       </c>
-      <c r="BP2" s="14" t="s">
+      <c r="CL2" t="s">
         <v>317</v>
       </c>
-      <c r="BQ2" s="14" t="s">
+      <c r="CM2" t="s">
+        <v>308</v>
+      </c>
+      <c r="CN2" t="s">
         <v>318</v>
       </c>
-      <c r="BR2" s="14" t="s">
+      <c r="CO2" t="s">
         <v>319</v>
       </c>
-      <c r="BS2" s="14" t="s">
+      <c r="CP2" t="s">
         <v>320</v>
       </c>
-      <c r="BT2" s="14" t="s">
+      <c r="CQ2" t="s">
         <v>321</v>
       </c>
-      <c r="BU2" s="14" t="s">
+      <c r="CR2" t="s">
         <v>322</v>
       </c>
-      <c r="BV2" s="14" t="s">
+      <c r="CS2" t="s">
         <v>323</v>
       </c>
-      <c r="BW2" s="14" t="s">
+      <c r="CT2" t="s">
         <v>324</v>
       </c>
-      <c r="BX2" s="14" t="s">
+      <c r="CU2" t="s">
         <v>325</v>
       </c>
-      <c r="BY2" s="14" t="s">
+      <c r="CV2" t="s">
         <v>326</v>
       </c>
-      <c r="BZ2" s="14" t="s">
+      <c r="CW2" t="s">
         <v>327</v>
       </c>
-      <c r="CA2" s="14" t="s">
+      <c r="CX2" t="s">
         <v>328</v>
       </c>
-      <c r="CB2" s="14" t="s">
+      <c r="CY2" t="s">
         <v>329</v>
       </c>
-      <c r="CC2" s="14" t="s">
+      <c r="CZ2" t="s">
         <v>330</v>
       </c>
-      <c r="CD2" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="CE2" s="14" t="s">
+      <c r="DA2" t="s">
         <v>331</v>
       </c>
-      <c r="CF2" s="14" t="s">
+      <c r="DB2" t="s">
         <v>332</v>
       </c>
-      <c r="CG2" s="14" t="s">
+      <c r="DC2" t="s">
         <v>333</v>
       </c>
-      <c r="CH2" s="14" t="s">
+      <c r="DD2" t="s">
         <v>334</v>
       </c>
-      <c r="CI2" s="14" t="s">
+      <c r="DE2" t="s">
         <v>335</v>
       </c>
-      <c r="CJ2" s="14" t="s">
+      <c r="DF2" t="s">
         <v>336</v>
       </c>
-      <c r="CK2" s="14" t="s">
+      <c r="DG2" t="s">
         <v>337</v>
       </c>
-      <c r="CL2" s="14" t="s">
+      <c r="DH2" t="s">
         <v>338</v>
       </c>
-      <c r="CM2" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="CN2" s="14" t="s">
+      <c r="DI2" t="s">
         <v>339</v>
       </c>
-      <c r="CO2" s="14" t="s">
+      <c r="DJ2" t="s">
         <v>340</v>
       </c>
-      <c r="CP2" s="14" t="s">
+      <c r="DK2" t="s">
         <v>341</v>
       </c>
-      <c r="CQ2" s="14" t="s">
+      <c r="DL2" t="s">
         <v>342</v>
       </c>
-      <c r="CR2" s="14" t="s">
+      <c r="DM2" t="s">
+        <v>366</v>
+      </c>
+      <c r="DN2" t="s">
         <v>343</v>
-      </c>
-      <c r="CS2" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="CT2" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="CU2" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="CV2" s="14" t="s">
-        <v>347</v>
-      </c>
-      <c r="CW2" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="CX2" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="CY2" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="CZ2" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="DA2" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="DB2" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="DC2" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="DD2" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="DE2" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="DF2" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="DG2" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="DH2" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="DI2" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="DJ2" s="14" t="s">
-        <v>361</v>
-      </c>
-      <c r="DK2" s="14" t="s">
-        <v>362</v>
-      </c>
-      <c r="DL2" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="DM2" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="DN2" s="14" t="s">
-        <v>364</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AMJ1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DO2:AMJ2">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="168"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>